<commit_message>
Luận theo cách cũ nhưng sẽ phải thêm lại key word trong file excel từng cung để luận
</commit_message>
<xml_diff>
--- a/LuanPhuMau.xlsx
+++ b/LuanPhuMau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3B11D12B-8811-485E-8EAB-9163078FE681}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC98B716-6195-4C08-8BAE-34EA51B5F407}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3326" uniqueCount="1663">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3328" uniqueCount="1664">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -5014,6 +5014,9 @@
   </si>
   <si>
     <t>Bạch Hổ, Thiên Hình đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Hữu Bật tọa thủ tại Phụ Mẫu</t>
   </si>
 </sst>
 </file>
@@ -5552,10 +5555,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B1663"/>
+  <dimension ref="A1:B1664"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1577" workbookViewId="0">
-      <selection activeCell="P1589" sqref="P1589"/>
+    <sheetView tabSelected="1" topLeftCell="A1652" workbookViewId="0">
+      <selection activeCell="B1664" sqref="B1664"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -18865,6 +18868,14 @@
       </c>
       <c r="B1663" t="s">
         <v>1662</v>
+      </c>
+    </row>
+    <row r="1664" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1664" t="s">
+        <v>1663</v>
+      </c>
+      <c r="B1664" t="s">
+        <v>1663</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Luận Cung Phụ Mẫu
</commit_message>
<xml_diff>
--- a/LuanPhuMau.xlsx
+++ b/LuanPhuMau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanTuVi\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2395DC4-BD9E-4B05-A333-C8A56E0BFA85}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34D9E98C-5FF7-4893-AE05-377C437ED69E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7624" uniqueCount="3734">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7706" uniqueCount="3775">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -11227,6 +11227,129 @@
   </si>
   <si>
     <t>Thai Phụ tọa thủ tại Huynh Đệ</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Tham Lang tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung Thiên Phủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thiên Tướng tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Thất Sát tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tử Vi đồng cung với Phá Quân tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Thiên Phủ tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Thiên Tướng tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Thất Sát tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Liêm Trinh đồng cung với Tham Lang tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung với Thiên Lương tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung với Thái Âm tại Phụ Mẫu ở Tý</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung với Thái Âm tại Phụ Mẫu ở Ngọ</t>
+  </si>
+  <si>
+    <t>Thiên Đồng đồng cung với Cự Môn tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Phụ Mẫu đồng cung Phá Quân</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Phụ Mẫu đồng cung Thất Sát</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Phụ Mẫu đồng cung Thiên Tướng</t>
+  </si>
+  <si>
+    <t>Vũ Khúc tọa thủ cung Phụ Mẫu đồng cung Thiên Phủ</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Phụ Mẫu ở Sửu đồng cung Thái Âm</t>
+  </si>
+  <si>
+    <t>Thái Dương tọa thủ cung Phụ Mẫu ở Mùi đồng cung Thái Âm</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Phụ Mẫu đồng cung Thái Âm ở Dần</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Phụ Mẫu đồng cung Thái Âm ở Thân</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Phụ Mẫu đồng cung Thiên Lương</t>
+  </si>
+  <si>
+    <t>Thiên Cơ tọa thủ cung Phụ Mẫu đồng cung Cự Môn</t>
+  </si>
+  <si>
+    <t>Tham Lang Vũ Khúc đồng cung tại cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thiên Lương đồng cung Thái Dương tại cung Phụ Mẫu ở Mão</t>
+  </si>
+  <si>
+    <t>Thiên Lương đồng cung Thái Dương tại cung Phụ Mẫu ở Dậu</t>
+  </si>
+  <si>
+    <t>Kình Dương, Liêm Trinh đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Kình Dương, Thất Sát đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Kình Dương, Tham Lang đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Đà La, Liêm Trinh đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Đà La, Thất Sát đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Đà La, Tham Lang đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung với Hỏa Tinh tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tham Lang đồng cung với Linh Tinh tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Phá Quân đồng cung với Hỏa Tinh tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Phá Quân đồng cung với Linh Tinh tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thái Âm, Hóa kỵ đồng cung tại Sửu</t>
+  </si>
+  <si>
+    <t>Thái Dương, Thái Âm, Hóa kỵ đồng cung tại Mùi</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La, Thiên Mã đồng cung tại Phụ Mẫu gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Kình Dương, Đà La, Thái Tuế đồng cung tại Phụ Mẫu gặp Hỏa Tinh, Linh Tinh</t>
+  </si>
+  <si>
+    <t>Đào Hoa, Hồng Loan, Thái Tuế đồng cung tại Phụ Mẫu</t>
   </si>
 </sst>
 </file>
@@ -11268,7 +11391,167 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="26">
+  <dxfs count="42">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <color rgb="FF9C0006"/>
@@ -11805,10 +12088,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:B3813"/>
+  <dimension ref="A1:B3855"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1652" workbookViewId="0">
-      <selection activeCell="P1658" sqref="P1658"/>
+    <sheetView tabSelected="1" topLeftCell="A3822" workbookViewId="0">
+      <selection activeCell="R3827" sqref="R3827"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -42312,63 +42595,419 @@
         <v>3612</v>
       </c>
     </row>
+    <row r="3815" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3815" t="s">
+        <v>3734</v>
+      </c>
+      <c r="B3815" t="s">
+        <v>3734</v>
+      </c>
+    </row>
+    <row r="3816" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3816" t="s">
+        <v>3735</v>
+      </c>
+      <c r="B3816" t="s">
+        <v>3735</v>
+      </c>
+    </row>
+    <row r="3817" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3817" t="s">
+        <v>3736</v>
+      </c>
+      <c r="B3817" t="s">
+        <v>3736</v>
+      </c>
+    </row>
+    <row r="3818" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3818" t="s">
+        <v>3737</v>
+      </c>
+      <c r="B3818" t="s">
+        <v>3737</v>
+      </c>
+    </row>
+    <row r="3819" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3819" t="s">
+        <v>3738</v>
+      </c>
+      <c r="B3819" t="s">
+        <v>3738</v>
+      </c>
+    </row>
+    <row r="3820" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3820" t="s">
+        <v>3739</v>
+      </c>
+      <c r="B3820" t="s">
+        <v>3739</v>
+      </c>
+    </row>
+    <row r="3821" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3821" t="s">
+        <v>3740</v>
+      </c>
+      <c r="B3821" t="s">
+        <v>3740</v>
+      </c>
+    </row>
+    <row r="3822" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3822" t="s">
+        <v>3741</v>
+      </c>
+      <c r="B3822" t="s">
+        <v>3741</v>
+      </c>
+    </row>
+    <row r="3823" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3823" t="s">
+        <v>3742</v>
+      </c>
+      <c r="B3823" t="s">
+        <v>3742</v>
+      </c>
+    </row>
+    <row r="3824" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3824" t="s">
+        <v>3743</v>
+      </c>
+      <c r="B3824" t="s">
+        <v>3743</v>
+      </c>
+    </row>
+    <row r="3825" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3825" t="s">
+        <v>3744</v>
+      </c>
+      <c r="B3825" t="s">
+        <v>3744</v>
+      </c>
+    </row>
+    <row r="3826" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3826" t="s">
+        <v>3745</v>
+      </c>
+      <c r="B3826" t="s">
+        <v>3745</v>
+      </c>
+    </row>
+    <row r="3827" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3827" t="s">
+        <v>3746</v>
+      </c>
+      <c r="B3827" t="s">
+        <v>3746</v>
+      </c>
+    </row>
+    <row r="3828" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3828" t="s">
+        <v>3747</v>
+      </c>
+      <c r="B3828" t="s">
+        <v>3747</v>
+      </c>
+    </row>
+    <row r="3829" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3829" t="s">
+        <v>3748</v>
+      </c>
+      <c r="B3829" t="s">
+        <v>3748</v>
+      </c>
+    </row>
+    <row r="3830" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3830" t="s">
+        <v>3749</v>
+      </c>
+      <c r="B3830" t="s">
+        <v>3749</v>
+      </c>
+    </row>
+    <row r="3831" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3831" t="s">
+        <v>3750</v>
+      </c>
+      <c r="B3831" t="s">
+        <v>3750</v>
+      </c>
+    </row>
+    <row r="3832" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3832" t="s">
+        <v>3751</v>
+      </c>
+      <c r="B3832" t="s">
+        <v>3751</v>
+      </c>
+    </row>
+    <row r="3833" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3833" t="s">
+        <v>3752</v>
+      </c>
+      <c r="B3833" t="s">
+        <v>3752</v>
+      </c>
+    </row>
+    <row r="3834" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3834" t="s">
+        <v>3753</v>
+      </c>
+      <c r="B3834" t="s">
+        <v>3753</v>
+      </c>
+    </row>
+    <row r="3835" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3835" t="s">
+        <v>3754</v>
+      </c>
+      <c r="B3835" t="s">
+        <v>3754</v>
+      </c>
+    </row>
+    <row r="3836" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3836" t="s">
+        <v>3755</v>
+      </c>
+      <c r="B3836" t="s">
+        <v>3755</v>
+      </c>
+    </row>
+    <row r="3837" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3837" t="s">
+        <v>3756</v>
+      </c>
+      <c r="B3837" t="s">
+        <v>3756</v>
+      </c>
+    </row>
+    <row r="3838" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3838" t="s">
+        <v>3757</v>
+      </c>
+      <c r="B3838" t="s">
+        <v>3757</v>
+      </c>
+    </row>
+    <row r="3839" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3839" t="s">
+        <v>3758</v>
+      </c>
+      <c r="B3839" t="s">
+        <v>3758</v>
+      </c>
+    </row>
+    <row r="3840" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3840" t="s">
+        <v>3759</v>
+      </c>
+      <c r="B3840" t="s">
+        <v>3759</v>
+      </c>
+    </row>
+    <row r="3841" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3841" t="s">
+        <v>3760</v>
+      </c>
+      <c r="B3841" t="s">
+        <v>3760</v>
+      </c>
+    </row>
+    <row r="3842" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3842" t="s">
+        <v>3761</v>
+      </c>
+      <c r="B3842" t="s">
+        <v>3761</v>
+      </c>
+    </row>
+    <row r="3843" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3843" t="s">
+        <v>3762</v>
+      </c>
+      <c r="B3843" t="s">
+        <v>3762</v>
+      </c>
+    </row>
+    <row r="3844" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3844" t="s">
+        <v>3763</v>
+      </c>
+      <c r="B3844" t="s">
+        <v>3763</v>
+      </c>
+    </row>
+    <row r="3845" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3845" t="s">
+        <v>3764</v>
+      </c>
+      <c r="B3845" t="s">
+        <v>3764</v>
+      </c>
+    </row>
+    <row r="3846" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3846" t="s">
+        <v>3765</v>
+      </c>
+      <c r="B3846" t="s">
+        <v>3765</v>
+      </c>
+    </row>
+    <row r="3847" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3847" t="s">
+        <v>3766</v>
+      </c>
+      <c r="B3847" t="s">
+        <v>3766</v>
+      </c>
+    </row>
+    <row r="3848" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3848" t="s">
+        <v>3767</v>
+      </c>
+      <c r="B3848" t="s">
+        <v>3767</v>
+      </c>
+    </row>
+    <row r="3849" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3849" t="s">
+        <v>3768</v>
+      </c>
+      <c r="B3849" t="s">
+        <v>3768</v>
+      </c>
+    </row>
+    <row r="3850" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3850" t="s">
+        <v>3769</v>
+      </c>
+      <c r="B3850" t="s">
+        <v>3769</v>
+      </c>
+    </row>
+    <row r="3851" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3851" t="s">
+        <v>3770</v>
+      </c>
+      <c r="B3851" t="s">
+        <v>3770</v>
+      </c>
+    </row>
+    <row r="3852" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3852" t="s">
+        <v>3771</v>
+      </c>
+      <c r="B3852" t="s">
+        <v>3771</v>
+      </c>
+    </row>
+    <row r="3853" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3853" t="s">
+        <v>3772</v>
+      </c>
+      <c r="B3853" t="s">
+        <v>3772</v>
+      </c>
+    </row>
+    <row r="3854" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3854" t="s">
+        <v>3773</v>
+      </c>
+      <c r="B3854" t="s">
+        <v>3773</v>
+      </c>
+    </row>
+    <row r="3855" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3855" t="s">
+        <v>3774</v>
+      </c>
+      <c r="B3855" t="s">
+        <v>3774</v>
+      </c>
+    </row>
   </sheetData>
   <dataConsolidate/>
   <conditionalFormatting sqref="A24">
-    <cfRule type="duplicateValues" dxfId="25" priority="74"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="75"/>
+    <cfRule type="duplicateValues" dxfId="41" priority="88"/>
+    <cfRule type="duplicateValues" dxfId="40" priority="89"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="23" priority="44"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="45"/>
+    <cfRule type="duplicateValues" dxfId="39" priority="58"/>
+    <cfRule type="duplicateValues" dxfId="38" priority="59"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
-    <cfRule type="duplicateValues" dxfId="21" priority="48"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="49"/>
+    <cfRule type="duplicateValues" dxfId="37" priority="62"/>
+    <cfRule type="duplicateValues" dxfId="36" priority="63"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A145:A208">
-    <cfRule type="duplicateValues" dxfId="19" priority="43"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="57"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A209:A1631 A1:A23 A25:A84 A143 A3682:A1048576">
-    <cfRule type="duplicateValues" dxfId="18" priority="83"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="85"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="97"/>
+    <cfRule type="duplicateValues" dxfId="33" priority="99"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1806:A1810 A3443:A3681">
-    <cfRule type="duplicateValues" dxfId="16" priority="5"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="32" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="31" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1811:A3340">
-    <cfRule type="duplicateValues" dxfId="14" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="30" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
-    <cfRule type="duplicateValues" dxfId="12" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="29" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="27"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="11" priority="8"/>
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="9" priority="10"/>
-    <cfRule type="duplicateValues" dxfId="8" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="25"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B208">
-    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B209:B1631 B1:B23 B25:B84 B143">
-    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
-    <cfRule type="duplicateValues" dxfId="5" priority="15"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="28"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="29"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1806:B1810 B3443:B3681">
-    <cfRule type="duplicateValues" dxfId="4" priority="2"/>
-    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="16"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="17"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1811:B3340">
-    <cfRule type="duplicateValues" dxfId="2" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="15"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B3682:B1048576">
-    <cfRule type="duplicateValues" dxfId="1" priority="24"/>
-    <cfRule type="duplicateValues" dxfId="0" priority="25"/>
+  <conditionalFormatting sqref="B3682:B3831 B3838 B3844:B3846 B3853:B1048576">
+    <cfRule type="duplicateValues" dxfId="17" priority="38"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="39"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3832:B3833">
+    <cfRule type="duplicateValues" dxfId="15" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3834:B3837">
+    <cfRule type="duplicateValues" dxfId="13" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="12"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3839:B3840">
+    <cfRule type="duplicateValues" dxfId="9" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="10"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3841:B3843">
+    <cfRule type="duplicateValues" dxfId="7" priority="7"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="8"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3847:B3848">
+    <cfRule type="duplicateValues" dxfId="5" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="6"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3849:B3850">
+    <cfRule type="duplicateValues" dxfId="3" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B3851:B3852">
+    <cfRule type="duplicateValues" dxfId="1" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Luận giải thích cung Phụ Mẫu
</commit_message>
<xml_diff>
--- a/LuanPhuMau.xlsx
+++ b/LuanPhuMau.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28925"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\App tu vi\LuanGiaiTuViBacPhai\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31B7AC66-8947-4456-8FB3-9410FB263AF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{290630E7-62C1-4D7D-9C76-2C3A9D783A02}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8829" uniqueCount="4469">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8859" uniqueCount="4534">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -13363,9 +13363,6 @@
 trong hai thân. </t>
   </si>
   <si>
-    <t xml:space="preserve">sớm xa cách hai thân. Trong nhà thiếu hòa khí. Có đi xa hay làm con nuôi họ khác mới tránh được mọi sự hình khắc. Nhưng dù sao chăng nữa, ít nhất là phải sớm lìa bỏ một trong hai thân. </t>
-  </si>
-  <si>
     <t>Sớm khắc một trong hai thân.</t>
   </si>
   <si>
@@ -13439,6 +13436,215 @@
   </si>
   <si>
     <t>Sớm khắc một trong hai thân. Nếu không, cũng phải xa cách hai thân. Cha mẹ bình thường. Trong nhà thiếu hòa khí nên làm con họ nhà khác.</t>
+  </si>
+  <si>
+    <t>Cha mẹ cũng bất hòa. Trong nhà có sự tranh chấp.</t>
+  </si>
+  <si>
+    <t>Cha mẹ cũng bất hòa. Trong nhà có sự tranh chấp. Cha mẹ giàu sang, nhưng không hợp tính với 
+con.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha mẹ cũng bất hòa. Trong nhà có sự tranh chấp. hai thân thường xa cách nhau. Nếu không, cũng sớm khắc một trong hai thân. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha mẹ cũng bất hòa. Trong nhà có sự tranh chấp. cha mẹ bỏ nhau, hay một còn một mất từ lúc con 
+còn ít tuổi. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân giàu có, qúy hiển và sống lâu, lợi ích cho 
+cha nhiều hơn cho mẹ. </t>
+  </si>
+  <si>
+    <t>Hai thân vất và, sớm khắc một trong hai thân. 
+Nên làm con nuôi họ khác.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sớm xa cách hai thân. Trong nhà thiếu hòa khí. Có đi xa hay làm con nuôi họ khác mới tránh được mọi sự hình khắc. Nhưng dù sao chăng nữa, ít nhất là phải sớm lìa bỏ một trong hai thân. </t>
+  </si>
+  <si>
+    <t>Thiên Tướng tọa thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Cha mẹ sống lâu.</t>
+  </si>
+  <si>
+    <t>Hai thân khá giả nhưng hay bất hòa.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân bình thường. Nên làm con nuôi họ khác 
+để tránh mọi hình khắc. </t>
+  </si>
+  <si>
+    <t>Cha mẹ nhân đức, giàu sang và sống lâu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân bình thường. Trong nhà thiếu hòa khí. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân bất hòa, hay xa cách nhau. Sớm lìa bỏ một 
+trong hai thân. Nếu không, cha mẹ và con cũng không thể sống chung với nhau lâu dài được. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân vất và, sớm khắc một trong hai thân. 
+Nên làm con nuôi họ khác. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha mẹ cũng bất hòa. Nếu không, cha mẹ và con cũng không hợp tính nhau. </t>
+  </si>
+  <si>
+    <t>Cha mẹ qúy hiến và sống lâu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha mẹ khá giả, nhưng sớm xa cách một trong hai 
+thân. </t>
+  </si>
+  <si>
+    <t>Cha mẹ túng thiếu, vất vả, thường mang cố tật, hay mắc ác bệnh. Nếu không, tất mắc nhiều tai họa. Sớm khắc một trong hai thân, cha mẹ và con cũng không thể sống chung với nhau lâu dài được. Nên làm con nuôi họ khác.</t>
+  </si>
+  <si>
+    <t>Phá Quân tọa thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sớm khắc một trong hai thân. Nếu không, hai thân cũng phải xa cách nhau. Trong nhà thiếu hòa khí. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha mẹ khá giá. </t>
+  </si>
+  <si>
+    <t>Cha mẹ bất hòa. Nên ở xa cha mẹ hay làm con nuôi họ khác.</t>
+  </si>
+  <si>
+    <t>Cha mẹ vất vả, không hợp tính với con. Sớm xa cách một trong hai thân.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cha mẹ và con cũng không hợp tính nhau </t>
+  </si>
+  <si>
+    <t>Cha mẹ và con cũng không hợp tính nhau</t>
+  </si>
+  <si>
+    <t>Hai thân hay mắc nạn, nhất là kiện cáo tù tội và thường phải xa cách nhau. Gia đình túng thiếu.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sớm xa cách hai thân, cha mẹ khó tránh được hình thương họa hại. </t>
+  </si>
+  <si>
+    <t>Cha hay mẹ là người hoang đàng chơi bời. Sớm xa cách một trong hai thân.</t>
+  </si>
+  <si>
+    <t>Bố mẹ giảm thọ. Trong nhà thiếu hòa khí.</t>
+  </si>
+  <si>
+    <t>Cha mẹ qúy hiến và giàu sang</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sớm khắc hai thân. Nếu không, cũng phải sớm xa cách, đi cư ngụ ở nơi đất khách quê người, cha mẹ thường mắc tai nạn bất kỳ, rất đáng lo ngại. 
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân cũng vất vả. Nếu không cũng bất hòa, cha 
+mẹ và con không hợp tính nhau. </t>
+  </si>
+  <si>
+    <t>Hai thân có học vấn</t>
+  </si>
+  <si>
+    <t>Cha mẹ thường là con trưởng. Nếu không, cũng đoạt trưởng gánh vác công việc gia đình có danh chức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân khá giả, nâng đỡ con trong nhiều công việc. Trong nhà có hòa khí. </t>
+  </si>
+  <si>
+    <t>Hai thân có của, nhưng con phá tán mất khá nhiều. Cha mẹ và con không hợp tính nhau. Nên ở xa cha mẹ.</t>
+  </si>
+  <si>
+    <t>Hai bố mẹ có của.</t>
+  </si>
+  <si>
+    <t>Bố mẹ có uy quyền, và nghiêm khắc với con cái.</t>
+  </si>
+  <si>
+    <t>Hai bố mẹ thông minh, nhân hậu, có danh chức</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân bất hòa. Nếu không, cha mẹ và con cũng không hợp tính nhau. </t>
+  </si>
+  <si>
+    <t>Thái Dương Thái Âm Hóa Kỵ đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Cha mẹ giàu sang</t>
+  </si>
+  <si>
+    <t>Hóa Kỵ Văn Xương, Văn Khúc đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Cha mẹ giảm thọ</t>
+  </si>
+  <si>
+    <t>Thiên Mã toạ thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Hai thân có danh giá, nhưng thường hay xa cách nhau.</t>
+  </si>
+  <si>
+    <t>Thiên Mã, Hóa Lộc đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Cha mẹ rất khá giả. Nhưng con nên ở xa cha mẹ.</t>
+  </si>
+  <si>
+    <t>Thiên Mã, Kình Đà đồng cung tại Phụ Mẫu</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Hai thân bất hòa, thường hay xung đột. Cha mẹ và con không hợp tính nhau. Nên ở xa cha mẹ. </t>
+  </si>
+  <si>
+    <t>Thiên Mã, Kình Đà đồng cung tại Phụ Mẫu gặp Hỏa Tinh, Linh Tinh, Địa Không, Địa Kiếp</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Chắc chắn là cha mẹ bỏ nhau. Nếu không, cũng một còn một mất, từ lúc con còn ít tuổi. Ngoài ra, cha mẹ thường mắc phải những tai nạn rất đáng lo ngại. </t>
+  </si>
+  <si>
+    <t>Thái Tuế toạ thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Tuế Phá toạ thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Trong nhà thiếu hòa khí, hay có sự tranh chấp. Cha mẹ và con không hợp tính nhau.</t>
+  </si>
+  <si>
+    <t>Thái Tuế toạ thủ cung Phụ Mẫu gặp Hỏa Tinh, Kình Dương, Đà La, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tất cha mẹ phải xa cách nhau. Gia đình ly tán. Ngoài ra, cha mẹ thường hay mắc tai họa, đáng lo ngại nhất là mắc kiện cáo. </t>
+  </si>
+  <si>
+    <t>Cô Thần toạ thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Quả Tú toạ thủ cung Phụ Mẫu</t>
+  </si>
+  <si>
+    <t>Hai thân không hợp tính nhau. Cha mẹ và con không thể ở gần nhau lâu được.</t>
+  </si>
+  <si>
+    <t>Cô Thần toạ thủ cung Phụ Mẫu gặp Hỏa Tinh, Kình Dương, Đà La, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Quả Tú toạ thủ cung Phụ Mẫu gặp Hỏa Tinh, Kình Dương, Hóa Kỵ</t>
+  </si>
+  <si>
+    <t>Hai thân không hợp tính nhau. Cha mẹ và con không thể ở gần nhau lâu được. Cô Thần lại gặp nhiều Sát tinh xâm phạm, tất sớm khắc một trong hai thân. Nên làm con nuôi họ khác</t>
+  </si>
+  <si>
+    <t>Hai thân không hợp tính nhau. Cha mẹ và con không thể ở gần nhau lâu 
+được. Quả Túlại gặp nhiều Sát tinh xâm phạm, tất sớm khắc một trong hai thân. Nên làm con nuôi họ khác</t>
+  </si>
+  <si>
+    <t>Cha hay mẹ thường là người tài hoa, phóng đãng. Đào Hồng Thái Tuế đồng cung, tất cha có vợ lẽ, ngoại tình, hay mẹ là người bất chính</t>
   </si>
 </sst>
 </file>
@@ -14153,10 +14359,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G4415"/>
+  <dimension ref="A2:G4430"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2542" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E2543" sqref="E2543"/>
+    <sheetView tabSelected="1" topLeftCell="A3754" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C3754" sqref="C3754"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -15242,7 +15448,7 @@
         <v>272</v>
       </c>
       <c r="B136" s="2" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -15282,7 +15488,7 @@
         <v>277</v>
       </c>
       <c r="B141" s="2" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -15322,7 +15528,7 @@
         <v>282</v>
       </c>
       <c r="B146" s="2" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -15362,7 +15568,7 @@
         <v>287</v>
       </c>
       <c r="B151" s="2" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -15402,7 +15608,7 @@
         <v>292</v>
       </c>
       <c r="B156" s="2" t="s">
-        <v>4450</v>
+        <v>4449</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -15538,7 +15744,7 @@
         <v>309</v>
       </c>
       <c r="B173" s="2" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -15570,7 +15776,7 @@
         <v>313</v>
       </c>
       <c r="B177" s="2" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -15602,7 +15808,7 @@
         <v>317</v>
       </c>
       <c r="B181" s="2" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -15634,7 +15840,7 @@
         <v>321</v>
       </c>
       <c r="B185" s="2" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -15666,7 +15872,7 @@
         <v>325</v>
       </c>
       <c r="B189" s="2" t="s">
-        <v>4451</v>
+        <v>4450</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -15793,8 +15999,8 @@
       <c r="A205" s="2" t="s">
         <v>341</v>
       </c>
-      <c r="B205" s="2" t="s">
-        <v>341</v>
+      <c r="B205" t="s">
+        <v>4493</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16026,7 +16232,7 @@
         <v>370</v>
       </c>
       <c r="B234" s="2" t="s">
-        <v>370</v>
+        <v>4492</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16146,7 +16352,7 @@
         <v>385</v>
       </c>
       <c r="B249" s="2" t="s">
-        <v>385</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16162,7 +16368,7 @@
         <v>387</v>
       </c>
       <c r="B251" s="2" t="s">
-        <v>387</v>
+        <v>4497</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16877,7 +17083,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="341" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="341" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A341" s="2" t="s">
         <v>477</v>
       </c>
@@ -16885,7 +17091,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="342" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="342" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A342" s="2" t="s">
         <v>478</v>
       </c>
@@ -17525,12 +17731,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="422" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="422" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A422" s="2" t="s">
         <v>553</v>
       </c>
       <c r="B422" s="2" t="s">
-        <v>553</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -17565,12 +17771,12 @@
         <v>557</v>
       </c>
     </row>
-    <row r="427" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="427" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A427" s="2" t="s">
         <v>558</v>
       </c>
       <c r="B427" s="2" t="s">
-        <v>558</v>
+        <v>4503</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -17770,7 +17976,7 @@
         <v>583</v>
       </c>
       <c r="B452" s="2" t="s">
-        <v>4458</v>
+        <v>4457</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -18165,7 +18371,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="502" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="502" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A502" s="2" t="s">
         <v>633</v>
       </c>
@@ -18517,7 +18723,7 @@
         <v>676</v>
       </c>
     </row>
-    <row r="546" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="546" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A546" s="2" t="s">
         <v>677</v>
       </c>
@@ -18901,7 +19107,7 @@
         <v>723</v>
       </c>
     </row>
-    <row r="594" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="594" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A594" s="2" t="s">
         <v>724</v>
       </c>
@@ -19493,20 +19699,20 @@
         <v>797</v>
       </c>
     </row>
-    <row r="668" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="668" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A668" s="2" t="s">
         <v>798</v>
       </c>
       <c r="B668" s="2" t="s">
-        <v>798</v>
-      </c>
-    </row>
-    <row r="669" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4500</v>
+      </c>
+    </row>
+    <row r="669" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A669" s="2" t="s">
         <v>799</v>
       </c>
       <c r="B669" s="2" t="s">
-        <v>799</v>
+        <v>4500</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
@@ -22026,7 +22232,7 @@
         <v>1113</v>
       </c>
       <c r="B984" s="2" t="s">
-        <v>1113</v>
+        <v>4505</v>
       </c>
     </row>
     <row r="985" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -22074,7 +22280,7 @@
         <v>1119</v>
       </c>
       <c r="B990" s="2" t="s">
-        <v>1119</v>
+        <v>4506</v>
       </c>
     </row>
     <row r="991" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -22146,7 +22352,7 @@
         <v>1128</v>
       </c>
       <c r="B999" s="2" t="s">
-        <v>1128</v>
+        <v>4507</v>
       </c>
     </row>
     <row r="1000" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -22197,12 +22403,12 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="1006" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1006" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1006" s="2" t="s">
         <v>1135</v>
       </c>
       <c r="B1006" s="2" t="s">
-        <v>1135</v>
+        <v>4508</v>
       </c>
     </row>
     <row r="1007" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -23394,7 +23600,7 @@
         <v>1284</v>
       </c>
       <c r="B1155" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="1156" spans="1:2" x14ac:dyDescent="0.25">
@@ -23538,7 +23744,7 @@
         <v>1287</v>
       </c>
       <c r="B1173" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="1174" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24245,7 +24451,7 @@
         <v>1371</v>
       </c>
     </row>
-    <row r="1262" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="1262" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1262" s="2" t="s">
         <v>1372</v>
       </c>
@@ -24434,7 +24640,7 @@
         <v>1395</v>
       </c>
       <c r="B1285" s="2" t="s">
-        <v>1395</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="1286" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24442,7 +24648,7 @@
         <v>1396</v>
       </c>
       <c r="B1286" s="2" t="s">
-        <v>1396</v>
+        <v>4473</v>
       </c>
     </row>
     <row r="1287" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24877,12 +25083,12 @@
         <v>1450</v>
       </c>
     </row>
-    <row r="1341" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1341" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1341" s="2" t="s">
         <v>1451</v>
       </c>
       <c r="B1341" s="2" t="s">
-        <v>1451</v>
+        <v>4483</v>
       </c>
     </row>
     <row r="1342" spans="1:2" x14ac:dyDescent="0.25">
@@ -25450,7 +25656,7 @@
         <v>1522</v>
       </c>
       <c r="B1412" s="2" t="s">
-        <v>1522</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1413" spans="1:2" x14ac:dyDescent="0.25">
@@ -25458,7 +25664,7 @@
         <v>1523</v>
       </c>
       <c r="B1413" s="2" t="s">
-        <v>1523</v>
+        <v>4501</v>
       </c>
     </row>
     <row r="1414" spans="1:2" x14ac:dyDescent="0.25">
@@ -26229,12 +26435,12 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="1510" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1510" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1510" s="2" t="s">
         <v>1620</v>
       </c>
       <c r="B1510" s="2" t="s">
-        <v>1620</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1511" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -26293,12 +26499,12 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="1518" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1518" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1518" s="2" t="s">
         <v>1628</v>
       </c>
       <c r="B1518" s="2" t="s">
-        <v>1628</v>
+        <v>4502</v>
       </c>
     </row>
     <row r="1519" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -26381,12 +26587,12 @@
         <v>1638</v>
       </c>
     </row>
-    <row r="1529" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1529" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1529" s="2" t="s">
         <v>1639</v>
       </c>
       <c r="B1529" s="2" t="s">
-        <v>1639</v>
+        <v>4504</v>
       </c>
     </row>
     <row r="1530" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -26629,12 +26835,12 @@
         <v>36</v>
       </c>
     </row>
-    <row r="1560" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1560" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1560" s="2" t="s">
         <v>37</v>
       </c>
       <c r="B1560" s="2" t="s">
-        <v>37</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="1561" spans="1:2" x14ac:dyDescent="0.25">
@@ -27274,7 +27480,7 @@
         <v>111</v>
       </c>
       <c r="B1640" s="2" t="s">
-        <v>4460</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="1641" spans="1:2" x14ac:dyDescent="0.25">
@@ -33938,7 +34144,7 @@
         <v>2362</v>
       </c>
       <c r="B2473" s="2" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="2474" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -33946,7 +34152,7 @@
         <v>2363</v>
       </c>
       <c r="B2474" s="2" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="2475" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -33954,7 +34160,7 @@
         <v>2364</v>
       </c>
       <c r="B2475" s="2" t="s">
-        <v>4453</v>
+        <v>4452</v>
       </c>
     </row>
     <row r="2476" spans="1:2" x14ac:dyDescent="0.25">
@@ -34042,7 +34248,7 @@
         <v>2375</v>
       </c>
       <c r="B2486" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2487" spans="1:2" x14ac:dyDescent="0.25">
@@ -34050,7 +34256,7 @@
         <v>2376</v>
       </c>
       <c r="B2487" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2488" spans="1:2" x14ac:dyDescent="0.25">
@@ -34058,7 +34264,7 @@
         <v>2377</v>
       </c>
       <c r="B2488" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2489" spans="1:2" x14ac:dyDescent="0.25">
@@ -34066,7 +34272,7 @@
         <v>2378</v>
       </c>
       <c r="B2489" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2490" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34074,7 +34280,7 @@
         <v>2379</v>
       </c>
       <c r="B2490" s="1" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="2491" spans="1:2" x14ac:dyDescent="0.25">
@@ -34082,7 +34288,7 @@
         <v>2380</v>
       </c>
       <c r="B2491" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2492" spans="1:2" x14ac:dyDescent="0.25">
@@ -34090,7 +34296,7 @@
         <v>2381</v>
       </c>
       <c r="B2492" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2493" spans="1:2" x14ac:dyDescent="0.25">
@@ -34098,7 +34304,7 @@
         <v>2382</v>
       </c>
       <c r="B2493" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2494" spans="1:2" x14ac:dyDescent="0.25">
@@ -34106,7 +34312,7 @@
         <v>2383</v>
       </c>
       <c r="B2494" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2495" spans="1:2" x14ac:dyDescent="0.25">
@@ -34114,7 +34320,7 @@
         <v>2384</v>
       </c>
       <c r="B2495" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2496" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34122,7 +34328,7 @@
         <v>2385</v>
       </c>
       <c r="B2496" s="1" t="s">
-        <v>4445</v>
+        <v>4444</v>
       </c>
     </row>
     <row r="2497" spans="1:2" x14ac:dyDescent="0.25">
@@ -34130,7 +34336,7 @@
         <v>2386</v>
       </c>
       <c r="B2497" s="1" t="s">
-        <v>4444</v>
+        <v>4443</v>
       </c>
     </row>
     <row r="2498" spans="1:2" x14ac:dyDescent="0.25">
@@ -34330,7 +34536,7 @@
         <v>2411</v>
       </c>
       <c r="B2522" s="2" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2523" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34338,7 +34544,7 @@
         <v>2412</v>
       </c>
       <c r="B2523" s="2" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="2524" spans="1:2" x14ac:dyDescent="0.25">
@@ -34346,7 +34552,7 @@
         <v>2413</v>
       </c>
       <c r="B2524" s="2" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2525" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34354,7 +34560,7 @@
         <v>2414</v>
       </c>
       <c r="B2525" s="2" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="2526" spans="1:2" x14ac:dyDescent="0.25">
@@ -34362,7 +34568,7 @@
         <v>2415</v>
       </c>
       <c r="B2526" s="2" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2527" spans="1:2" x14ac:dyDescent="0.25">
@@ -34370,7 +34576,7 @@
         <v>2416</v>
       </c>
       <c r="B2527" s="2" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2528" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34378,7 +34584,7 @@
         <v>2417</v>
       </c>
       <c r="B2528" s="2" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="2529" spans="1:2" x14ac:dyDescent="0.25">
@@ -34386,7 +34592,7 @@
         <v>2418</v>
       </c>
       <c r="B2529" s="2" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2530" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34394,7 +34600,7 @@
         <v>2419</v>
       </c>
       <c r="B2530" s="2" t="s">
-        <v>4461</v>
+        <v>4460</v>
       </c>
     </row>
     <row r="2531" spans="1:2" x14ac:dyDescent="0.25">
@@ -34402,7 +34608,7 @@
         <v>2420</v>
       </c>
       <c r="B2531" s="2" t="s">
-        <v>4459</v>
+        <v>4458</v>
       </c>
     </row>
     <row r="2532" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34410,7 +34616,7 @@
         <v>2421</v>
       </c>
       <c r="B2532" s="2" t="s">
-        <v>4460</v>
+        <v>4459</v>
       </c>
     </row>
     <row r="2533" spans="1:2" x14ac:dyDescent="0.25">
@@ -34490,7 +34696,7 @@
         <v>2431</v>
       </c>
       <c r="B2542" s="2" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="2543" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34498,7 +34704,7 @@
         <v>2432</v>
       </c>
       <c r="B2543" s="2" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="2544" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34506,7 +34712,7 @@
         <v>2433</v>
       </c>
       <c r="B2544" s="2" t="s">
-        <v>4463</v>
+        <v>4462</v>
       </c>
     </row>
     <row r="2545" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -34514,7 +34720,7 @@
         <v>2434</v>
       </c>
       <c r="B2545" s="2" t="s">
-        <v>4468</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="2546" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34522,7 +34728,7 @@
         <v>2435</v>
       </c>
       <c r="B2546" s="2" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="2547" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34530,7 +34736,7 @@
         <v>2436</v>
       </c>
       <c r="B2547" s="2" t="s">
-        <v>4467</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="2548" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34538,7 +34744,7 @@
         <v>2437</v>
       </c>
       <c r="B2548" s="2" t="s">
-        <v>4464</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="2549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34546,7 +34752,7 @@
         <v>2438</v>
       </c>
       <c r="B2549" s="2" t="s">
-        <v>4466</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="2550" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34554,7 +34760,7 @@
         <v>2439</v>
       </c>
       <c r="B2550" s="2" t="s">
-        <v>4464</v>
+        <v>4463</v>
       </c>
     </row>
     <row r="2551" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -34562,7 +34768,7 @@
         <v>2440</v>
       </c>
       <c r="B2551" s="2" t="s">
-        <v>4468</v>
+        <v>4467</v>
       </c>
     </row>
     <row r="2552" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34570,7 +34776,7 @@
         <v>2441</v>
       </c>
       <c r="B2552" s="2" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="2553" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34578,7 +34784,7 @@
         <v>2442</v>
       </c>
       <c r="B2553" s="2" t="s">
-        <v>4467</v>
+        <v>4466</v>
       </c>
     </row>
     <row r="2554" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34586,7 +34792,7 @@
         <v>2443</v>
       </c>
       <c r="B2554" s="2" t="s">
-        <v>4465</v>
+        <v>4464</v>
       </c>
     </row>
     <row r="2555" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34594,7 +34800,7 @@
         <v>2444</v>
       </c>
       <c r="B2555" s="2" t="s">
-        <v>4466</v>
+        <v>4465</v>
       </c>
     </row>
     <row r="2556" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34602,15 +34808,15 @@
         <v>2445</v>
       </c>
       <c r="B2556" s="2" t="s">
-        <v>4465</v>
-      </c>
-    </row>
-    <row r="2557" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4464</v>
+      </c>
+    </row>
+    <row r="2557" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2557" s="2" t="s">
         <v>2446</v>
       </c>
       <c r="B2557" s="2" t="s">
-        <v>2446</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="2558" spans="1:2" x14ac:dyDescent="0.25">
@@ -34618,7 +34824,7 @@
         <v>2447</v>
       </c>
       <c r="B2558" s="2" t="s">
-        <v>2447</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="2559" spans="1:2" x14ac:dyDescent="0.25">
@@ -34626,7 +34832,7 @@
         <v>2448</v>
       </c>
       <c r="B2559" s="2" t="s">
-        <v>2448</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="2560" spans="1:2" x14ac:dyDescent="0.25">
@@ -34634,31 +34840,31 @@
         <v>2449</v>
       </c>
       <c r="B2560" s="2" t="s">
-        <v>2449</v>
-      </c>
-    </row>
-    <row r="2561" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="2561" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2561" s="2" t="s">
         <v>2450</v>
       </c>
       <c r="B2561" s="2" t="s">
-        <v>2450</v>
-      </c>
-    </row>
-    <row r="2562" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="2562" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2562" s="2" t="s">
         <v>2451</v>
       </c>
       <c r="B2562" s="2" t="s">
-        <v>2451</v>
-      </c>
-    </row>
-    <row r="2563" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4470</v>
+      </c>
+    </row>
+    <row r="2563" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2563" s="2" t="s">
         <v>2452</v>
       </c>
       <c r="B2563" s="2" t="s">
-        <v>2452</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="2564" spans="1:2" x14ac:dyDescent="0.25">
@@ -34666,7 +34872,7 @@
         <v>2453</v>
       </c>
       <c r="B2564" s="2" t="s">
-        <v>2453</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="2565" spans="1:2" x14ac:dyDescent="0.25">
@@ -34674,7 +34880,7 @@
         <v>2454</v>
       </c>
       <c r="B2565" s="2" t="s">
-        <v>2454</v>
+        <v>4468</v>
       </c>
     </row>
     <row r="2566" spans="1:2" x14ac:dyDescent="0.25">
@@ -34682,23 +34888,23 @@
         <v>2455</v>
       </c>
       <c r="B2566" s="2" t="s">
-        <v>2455</v>
-      </c>
-    </row>
-    <row r="2567" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4468</v>
+      </c>
+    </row>
+    <row r="2567" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2567" s="2" t="s">
         <v>2456</v>
       </c>
       <c r="B2567" s="2" t="s">
-        <v>2456</v>
-      </c>
-    </row>
-    <row r="2568" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4471</v>
+      </c>
+    </row>
+    <row r="2568" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2568" s="2" t="s">
         <v>2457</v>
       </c>
       <c r="B2568" s="2" t="s">
-        <v>2457</v>
+        <v>4469</v>
       </c>
     </row>
     <row r="2569" spans="1:2" x14ac:dyDescent="0.25">
@@ -34714,7 +34920,7 @@
         <v>2459</v>
       </c>
       <c r="B2570" s="2" t="s">
-        <v>2459</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2571" spans="1:2" x14ac:dyDescent="0.25">
@@ -34725,12 +34931,12 @@
         <v>2460</v>
       </c>
     </row>
-    <row r="2572" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2572" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2572" s="2" t="s">
         <v>2461</v>
       </c>
       <c r="B2572" s="2" t="s">
-        <v>2461</v>
+        <v>4478</v>
       </c>
     </row>
     <row r="2573" spans="1:2" x14ac:dyDescent="0.25">
@@ -34746,7 +34952,7 @@
         <v>2463</v>
       </c>
       <c r="B2574" s="2" t="s">
-        <v>2463</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2575" spans="1:2" x14ac:dyDescent="0.25">
@@ -34762,7 +34968,7 @@
         <v>2465</v>
       </c>
       <c r="B2576" s="2" t="s">
-        <v>2465</v>
+        <v>4477</v>
       </c>
     </row>
     <row r="2577" spans="1:2" x14ac:dyDescent="0.25">
@@ -34786,15 +34992,15 @@
         <v>2468</v>
       </c>
       <c r="B2579" s="2" t="s">
-        <v>2468</v>
-      </c>
-    </row>
-    <row r="2580" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4477</v>
+      </c>
+    </row>
+    <row r="2580" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2580" s="2" t="s">
         <v>2469</v>
       </c>
       <c r="B2580" s="2" t="s">
-        <v>2469</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="2581" spans="1:2" x14ac:dyDescent="0.25">
@@ -34802,7 +35008,7 @@
         <v>2470</v>
       </c>
       <c r="B2581" s="2" t="s">
-        <v>2470</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="2582" spans="1:2" x14ac:dyDescent="0.25">
@@ -34834,7 +35040,7 @@
         <v>2474</v>
       </c>
       <c r="B2585" s="2" t="s">
-        <v>2474</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="2586" spans="1:2" x14ac:dyDescent="0.25">
@@ -34842,7 +35048,7 @@
         <v>2475</v>
       </c>
       <c r="B2586" s="2" t="s">
-        <v>2475</v>
+        <v>4479</v>
       </c>
     </row>
     <row r="2587" spans="1:2" x14ac:dyDescent="0.25">
@@ -34850,7 +35056,7 @@
         <v>2476</v>
       </c>
       <c r="B2587" s="2" t="s">
-        <v>2476</v>
+        <v>4480</v>
       </c>
     </row>
     <row r="2588" spans="1:2" x14ac:dyDescent="0.25">
@@ -34877,12 +35083,12 @@
         <v>2479</v>
       </c>
     </row>
-    <row r="2591" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2591" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2591" s="2" t="s">
         <v>2480</v>
       </c>
       <c r="B2591" s="2" t="s">
-        <v>2480</v>
+        <v>4481</v>
       </c>
     </row>
     <row r="2592" spans="1:2" x14ac:dyDescent="0.25">
@@ -34906,7 +35112,7 @@
         <v>2483</v>
       </c>
       <c r="B2594" s="2" t="s">
-        <v>2483</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="2595" spans="1:2" x14ac:dyDescent="0.25">
@@ -34917,28 +35123,28 @@
         <v>2484</v>
       </c>
     </row>
-    <row r="2596" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2596" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2596" s="2" t="s">
         <v>2485</v>
       </c>
       <c r="B2596" s="2" t="s">
-        <v>2485</v>
-      </c>
-    </row>
-    <row r="2597" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4486</v>
+      </c>
+    </row>
+    <row r="2597" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2597" s="2" t="s">
         <v>2486</v>
       </c>
       <c r="B2597" s="2" t="s">
-        <v>2486</v>
-      </c>
-    </row>
-    <row r="2598" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4485</v>
+      </c>
+    </row>
+    <row r="2598" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2598" s="2" t="s">
         <v>2487</v>
       </c>
       <c r="B2598" s="2" t="s">
-        <v>2487</v>
+        <v>4485</v>
       </c>
     </row>
     <row r="2599" spans="1:2" x14ac:dyDescent="0.25">
@@ -34954,7 +35160,7 @@
         <v>2489</v>
       </c>
       <c r="B2600" s="2" t="s">
-        <v>2489</v>
+        <v>4484</v>
       </c>
     </row>
     <row r="2601" spans="1:2" x14ac:dyDescent="0.25">
@@ -34965,12 +35171,12 @@
         <v>2490</v>
       </c>
     </row>
-    <row r="2602" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2602" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A2602" s="2" t="s">
         <v>2491</v>
       </c>
       <c r="B2602" s="2" t="s">
-        <v>2491</v>
+        <v>4486</v>
       </c>
     </row>
     <row r="2603" spans="1:2" x14ac:dyDescent="0.25">
@@ -34986,7 +35192,7 @@
         <v>2493</v>
       </c>
       <c r="B2604" s="2" t="s">
-        <v>2493</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="2605" spans="1:2" x14ac:dyDescent="0.25">
@@ -35001,8 +35207,8 @@
       <c r="A2606" s="2" t="s">
         <v>2495</v>
       </c>
-      <c r="B2606" s="2" t="s">
-        <v>2495</v>
+      <c r="B2606" t="s">
+        <v>4490</v>
       </c>
     </row>
     <row r="2607" spans="1:2" x14ac:dyDescent="0.25">
@@ -35017,8 +35223,8 @@
       <c r="A2608" s="2" t="s">
         <v>2497</v>
       </c>
-      <c r="B2608" s="2" t="s">
-        <v>2497</v>
+      <c r="B2608" t="s">
+        <v>4491</v>
       </c>
     </row>
     <row r="2609" spans="1:2" x14ac:dyDescent="0.25">
@@ -35034,7 +35240,7 @@
         <v>2499</v>
       </c>
       <c r="B2610" s="2" t="s">
-        <v>2499</v>
+        <v>4489</v>
       </c>
     </row>
     <row r="2611" spans="1:2" x14ac:dyDescent="0.25">
@@ -35049,8 +35255,8 @@
       <c r="A2612" s="2" t="s">
         <v>2501</v>
       </c>
-      <c r="B2612" s="2" t="s">
-        <v>2501</v>
+      <c r="B2612" t="s">
+        <v>4490</v>
       </c>
     </row>
     <row r="2613" spans="1:2" x14ac:dyDescent="0.25">
@@ -35065,8 +35271,8 @@
       <c r="A2614" s="2" t="s">
         <v>2503</v>
       </c>
-      <c r="B2614" s="2" t="s">
-        <v>2503</v>
+      <c r="B2614" t="s">
+        <v>4491</v>
       </c>
     </row>
     <row r="2615" spans="1:2" x14ac:dyDescent="0.25">
@@ -35562,7 +35768,7 @@
         <v>2565</v>
       </c>
       <c r="B2676" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2677" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35570,7 +35776,7 @@
         <v>2566</v>
       </c>
       <c r="B2677" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2678" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35578,7 +35784,7 @@
         <v>2567</v>
       </c>
       <c r="B2678" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2679" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35586,7 +35792,7 @@
         <v>2568</v>
       </c>
       <c r="B2679" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2680" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35594,7 +35800,7 @@
         <v>2569</v>
       </c>
       <c r="B2680" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2681" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35602,7 +35808,7 @@
         <v>2570</v>
       </c>
       <c r="B2681" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2682" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35610,7 +35816,7 @@
         <v>2571</v>
       </c>
       <c r="B2682" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2683" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35618,7 +35824,7 @@
         <v>2572</v>
       </c>
       <c r="B2683" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2684" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35626,7 +35832,7 @@
         <v>2573</v>
       </c>
       <c r="B2684" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2685" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35634,7 +35840,7 @@
         <v>2574</v>
       </c>
       <c r="B2685" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2686" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35642,7 +35848,7 @@
         <v>2575</v>
       </c>
       <c r="B2686" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2687" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -35650,7 +35856,7 @@
         <v>2576</v>
       </c>
       <c r="B2687" s="2" t="s">
-        <v>4462</v>
+        <v>4461</v>
       </c>
     </row>
     <row r="2688" spans="1:2" x14ac:dyDescent="0.25">
@@ -38245,12 +38451,12 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="3012" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3012" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3012" s="2" t="s">
         <v>2901</v>
       </c>
       <c r="B3012" s="2" t="s">
-        <v>2901</v>
+        <v>4472</v>
       </c>
     </row>
     <row r="3013" spans="1:2" x14ac:dyDescent="0.25">
@@ -38293,12 +38499,12 @@
         <v>2906</v>
       </c>
     </row>
-    <row r="3018" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3018" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3018" s="2" t="s">
         <v>2907</v>
       </c>
       <c r="B3018" s="2" t="s">
-        <v>2907</v>
+        <v>4482</v>
       </c>
     </row>
     <row r="3019" spans="1:2" x14ac:dyDescent="0.25">
@@ -43962,7 +44168,7 @@
         <v>3726</v>
       </c>
       <c r="B3726" s="2" t="s">
-        <v>4443</v>
+        <v>4474</v>
       </c>
     </row>
     <row r="3727" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -43970,7 +44176,7 @@
         <v>3727</v>
       </c>
       <c r="B3727" s="1" t="s">
-        <v>4449</v>
+        <v>4448</v>
       </c>
     </row>
     <row r="3728" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -43978,7 +44184,7 @@
         <v>3728</v>
       </c>
       <c r="B3728" s="1" t="s">
-        <v>4448</v>
+        <v>4447</v>
       </c>
     </row>
     <row r="3729" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43986,7 +44192,7 @@
         <v>3729</v>
       </c>
       <c r="B3729" s="1" t="s">
-        <v>4447</v>
+        <v>4446</v>
       </c>
     </row>
     <row r="3730" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -43994,7 +44200,7 @@
         <v>3730</v>
       </c>
       <c r="B3730" s="1" t="s">
-        <v>4446</v>
+        <v>4445</v>
       </c>
     </row>
     <row r="3731" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -44002,7 +44208,7 @@
         <v>3731</v>
       </c>
       <c r="B3731" s="2" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="3732" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -44010,7 +44216,7 @@
         <v>3732</v>
       </c>
       <c r="B3732" s="2" t="s">
-        <v>4452</v>
+        <v>4451</v>
       </c>
     </row>
     <row r="3733" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -44018,7 +44224,7 @@
         <v>3733</v>
       </c>
       <c r="B3733" s="2" t="s">
-        <v>4455</v>
+        <v>4454</v>
       </c>
     </row>
     <row r="3734" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -44026,7 +44232,7 @@
         <v>3734</v>
       </c>
       <c r="B3734" s="2" t="s">
-        <v>4454</v>
+        <v>4453</v>
       </c>
     </row>
     <row r="3735" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -44034,7 +44240,7 @@
         <v>3735</v>
       </c>
       <c r="B3735" s="2" t="s">
-        <v>4456</v>
+        <v>4455</v>
       </c>
     </row>
     <row r="3736" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -44042,7 +44248,7 @@
         <v>3736</v>
       </c>
       <c r="B3736" s="2" t="s">
-        <v>4457</v>
+        <v>4456</v>
       </c>
     </row>
     <row r="3737" spans="1:2" x14ac:dyDescent="0.25">
@@ -44069,28 +44275,28 @@
         <v>3739</v>
       </c>
     </row>
-    <row r="3740" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3740" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3740" s="2" t="s">
         <v>3740</v>
       </c>
       <c r="B3740" s="2" t="s">
-        <v>3740</v>
-      </c>
-    </row>
-    <row r="3741" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4494</v>
+      </c>
+    </row>
+    <row r="3741" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3741" s="2" t="s">
         <v>3741</v>
       </c>
       <c r="B3741" s="2" t="s">
-        <v>3741</v>
-      </c>
-    </row>
-    <row r="3742" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4495</v>
+      </c>
+    </row>
+    <row r="3742" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3742" s="2" t="s">
         <v>3742</v>
       </c>
       <c r="B3742" s="2" t="s">
-        <v>3742</v>
+        <v>4496</v>
       </c>
     </row>
     <row r="3743" spans="1:2" x14ac:dyDescent="0.25">
@@ -44122,7 +44328,7 @@
         <v>3746</v>
       </c>
       <c r="B3746" s="2" t="s">
-        <v>3746</v>
+        <v>4498</v>
       </c>
     </row>
     <row r="3747" spans="1:2" x14ac:dyDescent="0.25">
@@ -44130,23 +44336,23 @@
         <v>3747</v>
       </c>
       <c r="B3747" s="2" t="s">
-        <v>3747</v>
-      </c>
-    </row>
-    <row r="3748" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4498</v>
+      </c>
+    </row>
+    <row r="3748" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3748" s="2" t="s">
         <v>3748</v>
       </c>
       <c r="B3748" s="2" t="s">
-        <v>3748</v>
-      </c>
-    </row>
-    <row r="3749" spans="1:2" x14ac:dyDescent="0.25">
+        <v>4499</v>
+      </c>
+    </row>
+    <row r="3749" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A3749" s="2" t="s">
         <v>3749</v>
       </c>
       <c r="B3749" s="2" t="s">
-        <v>3749</v>
+        <v>4499</v>
       </c>
     </row>
     <row r="3750" spans="1:2" x14ac:dyDescent="0.25">
@@ -44181,12 +44387,12 @@
         <v>3753</v>
       </c>
     </row>
-    <row r="3754" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3754" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A3754" s="2" t="s">
         <v>3754</v>
       </c>
       <c r="B3754" s="2" t="s">
-        <v>3754</v>
+        <v>4533</v>
       </c>
     </row>
     <row r="3755" spans="1:2" x14ac:dyDescent="0.25">
@@ -49494,11 +49700,131 @@
       <c r="F4415" s="1"/>
       <c r="G4415" s="1"/>
     </row>
+    <row r="4416" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4416" s="1" t="s">
+        <v>4475</v>
+      </c>
+      <c r="B4416" s="1" t="s">
+        <v>4476</v>
+      </c>
+    </row>
+    <row r="4417" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4417" s="1" t="s">
+        <v>4487</v>
+      </c>
+      <c r="B4417" s="1" t="s">
+        <v>4488</v>
+      </c>
+    </row>
+    <row r="4418" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4418" s="1" t="s">
+        <v>4509</v>
+      </c>
+      <c r="B4418" s="1" t="s">
+        <v>4510</v>
+      </c>
+    </row>
+    <row r="4419" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4419" s="1" t="s">
+        <v>4511</v>
+      </c>
+      <c r="B4419" s="1" t="s">
+        <v>4512</v>
+      </c>
+    </row>
+    <row r="4420" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4420" s="1" t="s">
+        <v>4513</v>
+      </c>
+      <c r="B4420" s="1" t="s">
+        <v>4514</v>
+      </c>
+    </row>
+    <row r="4421" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4421" s="1" t="s">
+        <v>4515</v>
+      </c>
+      <c r="B4421" s="1" t="s">
+        <v>4516</v>
+      </c>
+    </row>
+    <row r="4422" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4422" s="1" t="s">
+        <v>4517</v>
+      </c>
+      <c r="B4422" s="1" t="s">
+        <v>4518</v>
+      </c>
+    </row>
+    <row r="4423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4423" s="1" t="s">
+        <v>4519</v>
+      </c>
+      <c r="B4423" s="1" t="s">
+        <v>4520</v>
+      </c>
+    </row>
+    <row r="4424" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4424" s="1" t="s">
+        <v>4522</v>
+      </c>
+      <c r="B4424" s="1" t="s">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="4425" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4425" s="1" t="s">
+        <v>4521</v>
+      </c>
+      <c r="B4425" s="1" t="s">
+        <v>4523</v>
+      </c>
+    </row>
+    <row r="4426" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A4426" s="1" t="s">
+        <v>4524</v>
+      </c>
+      <c r="B4426" s="1" t="s">
+        <v>4525</v>
+      </c>
+    </row>
+    <row r="4427" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4427" s="1" t="s">
+        <v>4526</v>
+      </c>
+      <c r="B4427" s="1" t="s">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="4428" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A4428" s="1" t="s">
+        <v>4527</v>
+      </c>
+      <c r="B4428" s="1" t="s">
+        <v>4528</v>
+      </c>
+    </row>
+    <row r="4429" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+      <c r="A4429" s="1" t="s">
+        <v>4529</v>
+      </c>
+      <c r="B4429" s="1" t="s">
+        <v>4531</v>
+      </c>
+    </row>
+    <row r="4430" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+      <c r="A4430" s="1" t="s">
+        <v>4530</v>
+      </c>
+      <c r="B4430" s="1" t="s">
+        <v>4532</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:G4415" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A4416:A1048576 A2:A4412">
-    <cfRule type="duplicateValues" dxfId="38" priority="13"/>
+  <conditionalFormatting sqref="A1:A1048576">
+    <cfRule type="duplicateValues" dxfId="38" priority="7"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A24">
     <cfRule type="duplicateValues" dxfId="37" priority="142"/>
@@ -49515,84 +49841,84 @@
   <conditionalFormatting sqref="A145:A208">
     <cfRule type="duplicateValues" dxfId="31" priority="111"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A6740:A1048576 A3660:A3834 A209:A1631 A2:A23 A25:A84 A143 A3897:A4195">
-    <cfRule type="duplicateValues" dxfId="30" priority="151"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="153"/>
+  <conditionalFormatting sqref="A1810:A3318">
+    <cfRule type="duplicateValues" dxfId="30" priority="367"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3421:A3659 A1805:A1809">
+    <cfRule type="duplicateValues" dxfId="29" priority="74"/>
     <cfRule type="duplicateValues" dxfId="28" priority="73"/>
-    <cfRule type="duplicateValues" dxfId="27" priority="74"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3835:A3896">
-    <cfRule type="duplicateValues" dxfId="26" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="53"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4416:A1048576 A2:A4412">
+    <cfRule type="duplicateValues" dxfId="26" priority="13"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4416:A1048576 A2:A4413">
+    <cfRule type="duplicateValues" dxfId="25" priority="11"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A4416:A1048576 A2:A4414">
+    <cfRule type="duplicateValues" dxfId="24" priority="9"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A6740:A1048576 A3660:A3834 A209:A1631 A2:A23 A25:A84 A143 A3897:A4195">
+    <cfRule type="duplicateValues" dxfId="23" priority="151"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="153"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1:C172 A174:C176 A173 C173 A178:C180 A177 C177 A182:C184 A181 C181 A186:C188 A185 C185 A189 C189 A2473:A2475 C2473:C2475 A190:C204 A2476:C2541 A2542:A2556 C2542:C2556 A2557:C2605 A2607:C2607 A2606 C2606 A2613:C2613 A2612 C2612 A2609:C2611 A2608 C2608 A2614 C2614 A205 C205 A2615:C1048576 A206:C2472">
+    <cfRule type="duplicateValues" dxfId="21" priority="6"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="25" priority="23"/>
-    <cfRule type="duplicateValues" dxfId="24" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="20" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="23" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="22" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="20"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B136">
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B141">
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="21" priority="21"/>
-    <cfRule type="duplicateValues" dxfId="20" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="14" priority="21"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="22"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B145:B172 B174:B176 B178:B180 B182:B184 B186:B188 B190:B208">
-    <cfRule type="duplicateValues" dxfId="19" priority="18"/>
+  <conditionalFormatting sqref="B145:B172 B174:B176 B178:B180 B182:B184 B186:B188 B190:B204 B206:B208">
+    <cfRule type="duplicateValues" dxfId="12" priority="18"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B6740:B1048576 B209:B1631 B2:B23 B25:B84 B143 B3897:B4195 B3660:B3834">
-    <cfRule type="duplicateValues" dxfId="18" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="17" priority="26"/>
+  <conditionalFormatting sqref="B1155">
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1173">
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1640">
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B1810:B2472 B2476:B2541 B2557:B2605 B2607 B2613 B2609:B2611 B2615:B3318">
+    <cfRule type="duplicateValues" dxfId="8" priority="369"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3421:B3659 B1805:B1809">
-    <cfRule type="duplicateValues" dxfId="16" priority="16"/>
-    <cfRule type="duplicateValues" dxfId="15" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="7" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3835:B3896">
-    <cfRule type="duplicateValues" dxfId="14" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="B6740:B1048576 B2:B23 B25:B84 B143 B3897:B4195 B3660:B3834 B209:B1631">
+    <cfRule type="duplicateValues" dxfId="4" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4413:W4413">
-    <cfRule type="duplicateValues" dxfId="13" priority="12"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4416:A1048576 A2:A4413">
-    <cfRule type="duplicateValues" dxfId="12" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4414:W4414">
-    <cfRule type="duplicateValues" dxfId="11" priority="10"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A4416:A1048576 A2:A4414">
-    <cfRule type="duplicateValues" dxfId="10" priority="9"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1810:A3318">
-    <cfRule type="duplicateValues" dxfId="9" priority="367"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1810:B2472 B2476:B2541 B2557:B3318">
-    <cfRule type="duplicateValues" dxfId="8" priority="369"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G4415:W4415">
-    <cfRule type="duplicateValues" dxfId="7" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:A1048576">
-    <cfRule type="duplicateValues" dxfId="6" priority="7"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1:C172 A174:C176 A173 C173 A178:C180 A177 C177 A182:C184 A181 C181 A186:C188 A185 C185 A189 C189 A2473:A2475 C2473:C2475 A190:C2472 A2476:C2541 A2557:C1048576 A2542:A2556 C2542:C2556">
-    <cfRule type="duplicateValues" dxfId="5" priority="6"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1155">
-    <cfRule type="duplicateValues" dxfId="4" priority="5"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1173">
-    <cfRule type="duplicateValues" dxfId="3" priority="4"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B136">
-    <cfRule type="duplicateValues" dxfId="2" priority="3"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B141">
-    <cfRule type="duplicateValues" dxfId="1" priority="2"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="B1640">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích phụ mẫu
</commit_message>
<xml_diff>
--- a/LuanPhuMau.xlsx
+++ b/LuanPhuMau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E8A588C6-A998-4BEF-8E6E-F82CD64F5627}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCF50030-5AD8-406D-AF1C-0CEA38C71733}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6764" uniqueCount="3495">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6765" uniqueCount="3496">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -10528,6 +10528,9 @@
   </si>
   <si>
     <t>Tả Phù tọa thủ tại Mệnh</t>
+  </si>
+  <si>
+    <t>Thái Dương và Cự Môn đồng cung tại Phụ Mẫu</t>
   </si>
 </sst>
 </file>
@@ -11245,10 +11248,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G3382"/>
+  <dimension ref="A2:G3383"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3085" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E3112" sqref="E3112"/>
+    <sheetView tabSelected="1" topLeftCell="A3374" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D3381" sqref="D3381"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -38325,6 +38328,11 @@
         <v>3484</v>
       </c>
     </row>
+    <row r="3383" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3383" s="1" t="s">
+        <v>3495</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A2:G3367" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
@@ -38336,8 +38344,8 @@
     <cfRule type="duplicateValues" dxfId="36" priority="143"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A85:A142">
-    <cfRule type="duplicateValues" dxfId="35" priority="112"/>
-    <cfRule type="duplicateValues" dxfId="34" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="35" priority="113"/>
+    <cfRule type="duplicateValues" dxfId="34" priority="112"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A144">
     <cfRule type="duplicateValues" dxfId="33" priority="116"/>
@@ -38346,84 +38354,84 @@
   <conditionalFormatting sqref="A145:A208">
     <cfRule type="duplicateValues" dxfId="31" priority="111"/>
   </conditionalFormatting>
+  <conditionalFormatting sqref="A1571:A2487">
+    <cfRule type="duplicateValues" dxfId="30" priority="5046"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="A1642:A1644 A1:C172 A174:C176 A173 C173 A178:C180 A177 C177 A182:C184 A181 C181 A186:C188 A185 C185 A189 C189 C1642:C1644 A190:C204 A1645:C1710 A1711:A1725 C1711:C1725 A1726:C1774 A1776:C1776 A1775 C1775 A1782:C1782 A1781 C1781 A1778:C1780 A1777 C1777 A1783 C1783 A205 C205 A1784:C1048576 A206:C1641">
+    <cfRule type="duplicateValues" dxfId="29" priority="6"/>
+  </conditionalFormatting>
   <conditionalFormatting sqref="A2590:A2828 A1570">
-    <cfRule type="duplicateValues" dxfId="30" priority="73"/>
-    <cfRule type="duplicateValues" dxfId="29" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="28" priority="74"/>
+    <cfRule type="duplicateValues" dxfId="27" priority="73"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3004:A3065">
-    <cfRule type="duplicateValues" dxfId="28" priority="53"/>
+    <cfRule type="duplicateValues" dxfId="26" priority="53"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3368:A1048576 A2:A3364">
-    <cfRule type="duplicateValues" dxfId="27" priority="13"/>
+    <cfRule type="duplicateValues" dxfId="25" priority="13"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3368:A1048576 A2:A3365">
-    <cfRule type="duplicateValues" dxfId="26" priority="11"/>
+    <cfRule type="duplicateValues" dxfId="24" priority="11"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A3368:A1048576 A2:A3366">
-    <cfRule type="duplicateValues" dxfId="25" priority="9"/>
+    <cfRule type="duplicateValues" dxfId="23" priority="9"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A5692:A1048576 A2829:A3003 A209:A1551 A2:A23 A25:A84 A143 A3066:A3147">
-    <cfRule type="duplicateValues" dxfId="24" priority="151"/>
-    <cfRule type="duplicateValues" dxfId="23" priority="153"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1642:A1644 A1:C172 A174:C176 A173 C173 A178:C180 A177 C177 A182:C184 A181 C181 A186:C188 A185 C185 A189 C189 C1642:C1644 A190:C204 A1645:C1710 A1711:A1725 C1711:C1725 A1726:C1774 A1776:C1776 A1775 C1775 A1782:C1782 A1781 C1781 A1778:C1780 A1777 C1777 A1783 C1783 A205 C205 A1784:C1048576 A206:C1641">
-    <cfRule type="duplicateValues" dxfId="22" priority="6"/>
+    <cfRule type="duplicateValues" dxfId="22" priority="151"/>
+    <cfRule type="duplicateValues" dxfId="21" priority="153"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B24">
-    <cfRule type="duplicateValues" dxfId="21" priority="23"/>
     <cfRule type="duplicateValues" dxfId="20" priority="24"/>
+    <cfRule type="duplicateValues" dxfId="19" priority="23"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B85:B142">
-    <cfRule type="duplicateValues" dxfId="19" priority="19"/>
-    <cfRule type="duplicateValues" dxfId="18" priority="20"/>
+    <cfRule type="duplicateValues" dxfId="18" priority="19"/>
+    <cfRule type="duplicateValues" dxfId="17" priority="20"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B136">
-    <cfRule type="duplicateValues" dxfId="17" priority="3"/>
+    <cfRule type="duplicateValues" dxfId="16" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B141">
-    <cfRule type="duplicateValues" dxfId="16" priority="2"/>
+    <cfRule type="duplicateValues" dxfId="15" priority="2"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B144">
-    <cfRule type="duplicateValues" dxfId="15" priority="21"/>
     <cfRule type="duplicateValues" dxfId="14" priority="22"/>
+    <cfRule type="duplicateValues" dxfId="13" priority="21"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B145:B172 B174:B176 B178:B180 B182:B184 B186:B188 B190:B204 B206:B208">
-    <cfRule type="duplicateValues" dxfId="13" priority="18"/>
+    <cfRule type="duplicateValues" dxfId="12" priority="18"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1155">
-    <cfRule type="duplicateValues" dxfId="12" priority="5"/>
+    <cfRule type="duplicateValues" dxfId="11" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1156">
-    <cfRule type="duplicateValues" dxfId="11" priority="4"/>
+    <cfRule type="duplicateValues" dxfId="10" priority="4"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1553">
-    <cfRule type="duplicateValues" dxfId="10" priority="1"/>
+    <cfRule type="duplicateValues" dxfId="9" priority="1"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B1645:B1710 B1571:B1641 B1726:B1774 B1776 B1782 B1778:B1780 B1784:B2487">
-    <cfRule type="duplicateValues" dxfId="9" priority="369"/>
+    <cfRule type="duplicateValues" dxfId="8" priority="369"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B2590:B2828 B1570">
-    <cfRule type="duplicateValues" dxfId="8" priority="16"/>
     <cfRule type="duplicateValues" dxfId="7" priority="17"/>
+    <cfRule type="duplicateValues" dxfId="6" priority="16"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B3004:B3065">
-    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
+    <cfRule type="duplicateValues" dxfId="5" priority="14"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="B5692:B1048576 B2:B23 B25:B84 B143 B3066:B3147 B2829:B3003 B209:B1551">
-    <cfRule type="duplicateValues" dxfId="5" priority="25"/>
-    <cfRule type="duplicateValues" dxfId="4" priority="26"/>
+    <cfRule type="duplicateValues" dxfId="4" priority="25"/>
+    <cfRule type="duplicateValues" dxfId="3" priority="26"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3365:W3365">
-    <cfRule type="duplicateValues" dxfId="3" priority="12"/>
+    <cfRule type="duplicateValues" dxfId="2" priority="12"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3366:W3366">
-    <cfRule type="duplicateValues" dxfId="2" priority="10"/>
+    <cfRule type="duplicateValues" dxfId="1" priority="10"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="G3367:W3367">
-    <cfRule type="duplicateValues" dxfId="1" priority="8"/>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="A1571:A2487">
-    <cfRule type="duplicateValues" dxfId="0" priority="5046"/>
+    <cfRule type="duplicateValues" dxfId="0" priority="8"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Giải thích phụ tinh tại Phụ Mẫu
</commit_message>
<xml_diff>
--- a/LuanPhuMau.xlsx
+++ b/LuanPhuMau.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hieuxnk1\Documents\App_tu_vi-main\LuanGiaiTuViBacPhai\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30D7984C-93A7-49F0-B3AB-BFE7A0C62A89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{10DE1F5A-A0F6-4883-9FA3-1385C7683B48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$G$3189</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$2:$G$3202</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6431" uniqueCount="3388">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6425" uniqueCount="3389">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -4800,9 +4800,6 @@
     <t>Quan Phù tọa thủ tại Phụ Mẫu</t>
   </si>
   <si>
-    <t>Quý Nhân tọa thủ tại Phụ Mẫu</t>
-  </si>
-  <si>
     <t>Tử Vi tọa thủ tại Tý</t>
   </si>
   <si>
@@ -8976,9 +8973,6 @@
     <t>Văn Tinh tọa thủ tại Phụ Mẫu</t>
   </si>
   <si>
-    <t>Phúc Đức tọa thủ tại Phúc Đức</t>
-  </si>
-  <si>
     <t>(Hóa Khoa - ĐV) tọa thủ tại Phụ Mẫu</t>
   </si>
   <si>
@@ -9016,9 +9010,6 @@
   </si>
   <si>
     <t>Đẩu Quân tọa thủ tại Phụ Mẫu</t>
-  </si>
-  <si>
-    <t>Kình Dương (ĐV) tọa thủ tại Mệnh</t>
   </si>
   <si>
     <t>Kình Dương (ĐV) tọa thủ tại Phụ Mẫu</t>
@@ -10208,6 +10199,18 @@
   </si>
   <si>
     <t>Cha mẹ là những người có sức khỏe, cao lớn, chịu khó làm ăn không nề hà việc lớn bé.</t>
+  </si>
+  <si>
+    <t>Mẹ cha là người thanh lịch, có học thức, hiền lành, đức độ.</t>
+  </si>
+  <si>
+    <t>Cha mẹ sẽ có tí đường công danh, ít nhiều uy lực uy quyền, lời ăn tiếng nói với tổ chức xã hội ở bên ngoài. Cha mẹ cơ bản sẽ khá giả</t>
+  </si>
+  <si>
+    <t>Giúp tăng thọ trường, đem lại may lắm cho cha mẹ. Cha mẹ là người đẹp đẽ, thanh cao, ôn hòa, có tài chính, điền sản, người hay làm phước thiện.</t>
+  </si>
+  <si>
+    <t>Cha mẹ có chức vị, có học thức và bằng cấp cao. Cha mẹ hay được khen thưởng, vinh danh, thăng cấp. Người có nhiều bằng sắc, giấy công nhận. Con cháu sau này cũng sẽ nhiều bằng cấp, học vị cao.</t>
   </si>
 </sst>
 </file>
@@ -10925,10 +10928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A2:G3205"/>
+  <dimension ref="A2:G3202"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1590" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1602" sqref="C1602"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -10951,7 +10954,7 @@
         <v>26</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>3191</v>
+        <v>3188</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10959,7 +10962,7 @@
         <v>27</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>3192</v>
+        <v>3189</v>
       </c>
     </row>
     <row r="5" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10967,7 +10970,7 @@
         <v>28</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>3193</v>
+        <v>3190</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10975,7 +10978,7 @@
         <v>29</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>3194</v>
+        <v>3191</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -10983,7 +10986,7 @@
         <v>31</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>3195</v>
+        <v>3192</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -11004,10 +11007,10 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
-        <v>3196</v>
+        <v>3193</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>3197</v>
+        <v>3194</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -12015,7 +12018,7 @@
         <v>157</v>
       </c>
       <c r="B136" s="1" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="137" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12055,7 +12058,7 @@
         <v>162</v>
       </c>
       <c r="B141" s="1" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="142" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12095,7 +12098,7 @@
         <v>167</v>
       </c>
       <c r="B146" s="1" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="147" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12135,7 +12138,7 @@
         <v>172</v>
       </c>
       <c r="B151" s="1" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="152" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12175,7 +12178,7 @@
         <v>177</v>
       </c>
       <c r="B156" s="1" t="s">
-        <v>3223</v>
+        <v>3220</v>
       </c>
     </row>
     <row r="157" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -12311,7 +12314,7 @@
         <v>194</v>
       </c>
       <c r="B173" s="1" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="174" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -12343,7 +12346,7 @@
         <v>198</v>
       </c>
       <c r="B177" s="1" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="178" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -12375,7 +12378,7 @@
         <v>202</v>
       </c>
       <c r="B181" s="1" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="182" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -12407,7 +12410,7 @@
         <v>206</v>
       </c>
       <c r="B185" s="1" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="186" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -12439,7 +12442,7 @@
         <v>210</v>
       </c>
       <c r="B189" s="1" t="s">
-        <v>3224</v>
+        <v>3221</v>
       </c>
     </row>
     <row r="190" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -12567,7 +12570,7 @@
         <v>226</v>
       </c>
       <c r="B205" s="3" t="s">
-        <v>3267</v>
+        <v>3264</v>
       </c>
     </row>
     <row r="206" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12799,7 +12802,7 @@
         <v>255</v>
       </c>
       <c r="B234" s="1" t="s">
-        <v>3266</v>
+        <v>3263</v>
       </c>
     </row>
     <row r="235" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12919,7 +12922,7 @@
         <v>270</v>
       </c>
       <c r="B249" s="1" t="s">
-        <v>3271</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="250" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -12935,7 +12938,7 @@
         <v>272</v>
       </c>
       <c r="B251" s="1" t="s">
-        <v>3271</v>
+        <v>3268</v>
       </c>
     </row>
     <row r="252" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -14303,7 +14306,7 @@
         <v>438</v>
       </c>
       <c r="B422" s="1" t="s">
-        <v>3277</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="423" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -14343,7 +14346,7 @@
         <v>443</v>
       </c>
       <c r="B427" s="1" t="s">
-        <v>3277</v>
+        <v>3274</v>
       </c>
     </row>
     <row r="428" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -14543,7 +14546,7 @@
         <v>468</v>
       </c>
       <c r="B452" s="1" t="s">
-        <v>3231</v>
+        <v>3228</v>
       </c>
     </row>
     <row r="453" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16271,7 +16274,7 @@
         <v>683</v>
       </c>
       <c r="B668" s="1" t="s">
-        <v>3274</v>
+        <v>3271</v>
       </c>
     </row>
     <row r="669" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16279,7 +16282,7 @@
         <v>684</v>
       </c>
       <c r="B669" s="1" t="s">
-        <v>3274</v>
+        <v>3271</v>
       </c>
     </row>
     <row r="670" spans="1:2" x14ac:dyDescent="0.25">
@@ -18799,7 +18802,7 @@
         <v>998</v>
       </c>
       <c r="B984" s="1" t="s">
-        <v>3279</v>
+        <v>3276</v>
       </c>
     </row>
     <row r="985" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -18847,7 +18850,7 @@
         <v>1004</v>
       </c>
       <c r="B990" s="1" t="s">
-        <v>3280</v>
+        <v>3277</v>
       </c>
     </row>
     <row r="991" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -18919,7 +18922,7 @@
         <v>1013</v>
       </c>
       <c r="B999" s="1" t="s">
-        <v>3281</v>
+        <v>3278</v>
       </c>
     </row>
     <row r="1000" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -18975,7 +18978,7 @@
         <v>1020</v>
       </c>
       <c r="B1006" s="1" t="s">
-        <v>3282</v>
+        <v>3279</v>
       </c>
     </row>
     <row r="1007" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -20151,7 +20154,7 @@
         <v>1167</v>
       </c>
       <c r="B1153" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1154" spans="1:2" x14ac:dyDescent="0.25">
@@ -20159,7 +20162,7 @@
         <v>1168</v>
       </c>
       <c r="B1154" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1155" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -21047,7 +21050,7 @@
         <v>1276</v>
       </c>
       <c r="B1265" s="1" t="s">
-        <v>3246</v>
+        <v>3243</v>
       </c>
     </row>
     <row r="1266" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -21055,7 +21058,7 @@
         <v>1277</v>
       </c>
       <c r="B1266" s="1" t="s">
-        <v>3247</v>
+        <v>3244</v>
       </c>
     </row>
     <row r="1267" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -21495,7 +21498,7 @@
         <v>1332</v>
       </c>
       <c r="B1321" s="1" t="s">
-        <v>3257</v>
+        <v>3254</v>
       </c>
     </row>
     <row r="1322" spans="1:2" x14ac:dyDescent="0.25">
@@ -22063,7 +22066,7 @@
         <v>1403</v>
       </c>
       <c r="B1392" s="1" t="s">
-        <v>3275</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="1393" spans="1:2" x14ac:dyDescent="0.25">
@@ -22071,7 +22074,7 @@
         <v>1404</v>
       </c>
       <c r="B1393" s="1" t="s">
-        <v>3275</v>
+        <v>3272</v>
       </c>
     </row>
     <row r="1394" spans="1:2" x14ac:dyDescent="0.25">
@@ -22847,7 +22850,7 @@
         <v>1501</v>
       </c>
       <c r="B1490" s="1" t="s">
-        <v>3276</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="1491" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -22911,7 +22914,7 @@
         <v>1509</v>
       </c>
       <c r="B1498" s="1" t="s">
-        <v>3276</v>
+        <v>3273</v>
       </c>
     </row>
     <row r="1499" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -22999,7 +23002,7 @@
         <v>1520</v>
       </c>
       <c r="B1509" s="1" t="s">
-        <v>3278</v>
+        <v>3275</v>
       </c>
     </row>
     <row r="1510" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -23175,7 +23178,7 @@
         <v>12</v>
       </c>
       <c r="B1531" s="1" t="s">
-        <v>3308</v>
+        <v>3305</v>
       </c>
     </row>
     <row r="1532" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -23183,7 +23186,7 @@
         <v>13</v>
       </c>
       <c r="B1532" s="1" t="s">
-        <v>3309</v>
+        <v>3306</v>
       </c>
     </row>
     <row r="1533" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -23191,7 +23194,7 @@
         <v>14</v>
       </c>
       <c r="B1533" s="1" t="s">
-        <v>3310</v>
+        <v>3307</v>
       </c>
     </row>
     <row r="1534" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23199,10 +23202,10 @@
         <v>15</v>
       </c>
       <c r="B1534" s="1" t="s">
-        <v>3311</v>
+        <v>3308</v>
       </c>
       <c r="C1534" s="1" t="s">
-        <v>3312</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="1535" spans="1:3" x14ac:dyDescent="0.25">
@@ -23210,10 +23213,10 @@
         <v>16</v>
       </c>
       <c r="B1535" s="1" t="s">
-        <v>3313</v>
+        <v>3310</v>
       </c>
       <c r="C1535" s="1" t="s">
-        <v>3367</v>
+        <v>3364</v>
       </c>
     </row>
     <row r="1536" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23221,7 +23224,7 @@
         <v>17</v>
       </c>
       <c r="B1536" s="1" t="s">
-        <v>3314</v>
+        <v>3311</v>
       </c>
     </row>
     <row r="1537" spans="1:3" x14ac:dyDescent="0.25">
@@ -23237,7 +23240,7 @@
         <v>19</v>
       </c>
       <c r="B1538" s="1" t="s">
-        <v>3315</v>
+        <v>3312</v>
       </c>
     </row>
     <row r="1539" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -23245,7 +23248,7 @@
         <v>20</v>
       </c>
       <c r="B1539" s="1" t="s">
-        <v>3252</v>
+        <v>3249</v>
       </c>
     </row>
     <row r="1540" spans="1:3" x14ac:dyDescent="0.25">
@@ -23261,7 +23264,7 @@
         <v>22</v>
       </c>
       <c r="B1541" s="1" t="s">
-        <v>3233</v>
+        <v>3230</v>
       </c>
     </row>
     <row r="1542" spans="1:3" x14ac:dyDescent="0.25">
@@ -23293,7 +23296,7 @@
         <v>1543</v>
       </c>
       <c r="B1545" s="1" t="s">
-        <v>3333</v>
+        <v>3330</v>
       </c>
     </row>
     <row r="1546" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23301,7 +23304,7 @@
         <v>1544</v>
       </c>
       <c r="B1546" s="1" t="s">
-        <v>3334</v>
+        <v>3331</v>
       </c>
     </row>
     <row r="1547" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23309,7 +23312,7 @@
         <v>1545</v>
       </c>
       <c r="B1547" s="1" t="s">
-        <v>3334</v>
+        <v>3331</v>
       </c>
     </row>
     <row r="1548" spans="1:3" ht="120" x14ac:dyDescent="0.25">
@@ -23317,7 +23320,7 @@
         <v>1546</v>
       </c>
       <c r="B1548" s="1" t="s">
-        <v>3335</v>
+        <v>3332</v>
       </c>
     </row>
     <row r="1549" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -23325,7 +23328,7 @@
         <v>1547</v>
       </c>
       <c r="B1549" s="1" t="s">
-        <v>3336</v>
+        <v>3333</v>
       </c>
     </row>
     <row r="1550" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23333,7 +23336,7 @@
         <v>1548</v>
       </c>
       <c r="B1550" s="1" t="s">
-        <v>3337</v>
+        <v>3334</v>
       </c>
     </row>
     <row r="1551" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -23341,7 +23344,7 @@
         <v>1549</v>
       </c>
       <c r="B1551" s="1" t="s">
-        <v>3338</v>
+        <v>3335</v>
       </c>
     </row>
     <row r="1552" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23349,10 +23352,10 @@
         <v>1550</v>
       </c>
       <c r="B1552" s="1" t="s">
-        <v>3311</v>
+        <v>3308</v>
       </c>
       <c r="C1552" s="1" t="s">
-        <v>3312</v>
+        <v>3309</v>
       </c>
     </row>
     <row r="1553" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -23360,7 +23363,7 @@
         <v>1551</v>
       </c>
       <c r="B1553" s="1" t="s">
-        <v>3339</v>
+        <v>3336</v>
       </c>
     </row>
     <row r="1554" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -23368,7 +23371,7 @@
         <v>1552</v>
       </c>
       <c r="B1554" s="1" t="s">
-        <v>3340</v>
+        <v>3337</v>
       </c>
     </row>
     <row r="1555" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -23376,7 +23379,7 @@
         <v>1553</v>
       </c>
       <c r="B1555" s="1" t="s">
-        <v>3317</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="1556" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -23384,7 +23387,7 @@
         <v>1554</v>
       </c>
       <c r="B1556" s="1" t="s">
-        <v>3317</v>
+        <v>3314</v>
       </c>
     </row>
     <row r="1557" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -23392,7 +23395,7 @@
         <v>1555</v>
       </c>
       <c r="B1557" s="1" t="s">
-        <v>3318</v>
+        <v>3315</v>
       </c>
     </row>
     <row r="1558" spans="1:4" ht="45" x14ac:dyDescent="0.25">
@@ -23400,7 +23403,7 @@
         <v>1556</v>
       </c>
       <c r="B1558" s="1" t="s">
-        <v>3319</v>
+        <v>3316</v>
       </c>
     </row>
     <row r="1559" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -23408,10 +23411,10 @@
         <v>1557</v>
       </c>
       <c r="B1559" s="1" t="s">
-        <v>3321</v>
+        <v>3318</v>
       </c>
       <c r="C1559" s="1" t="s">
-        <v>3322</v>
+        <v>3319</v>
       </c>
     </row>
     <row r="1560" spans="1:4" ht="120" x14ac:dyDescent="0.25">
@@ -23419,7 +23422,7 @@
         <v>1558</v>
       </c>
       <c r="B1560" s="1" t="s">
-        <v>3320</v>
+        <v>3317</v>
       </c>
     </row>
     <row r="1561" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -23427,7 +23430,7 @@
         <v>1559</v>
       </c>
       <c r="B1561" s="1" t="s">
-        <v>3323</v>
+        <v>3320</v>
       </c>
     </row>
     <row r="1562" spans="1:4" ht="210" x14ac:dyDescent="0.25">
@@ -23435,13 +23438,13 @@
         <v>1560</v>
       </c>
       <c r="B1562" s="1" t="s">
-        <v>3324</v>
+        <v>3321</v>
       </c>
       <c r="C1562" s="1" t="s">
+        <v>3322</v>
+      </c>
+      <c r="D1562" s="1" t="s">
         <v>3325</v>
-      </c>
-      <c r="D1562" s="1" t="s">
-        <v>3328</v>
       </c>
     </row>
     <row r="1563" spans="1:4" ht="75" x14ac:dyDescent="0.25">
@@ -23449,10 +23452,10 @@
         <v>1561</v>
       </c>
       <c r="B1563" s="1" t="s">
-        <v>3326</v>
+        <v>3323</v>
       </c>
       <c r="C1563" s="1" t="s">
-        <v>3327</v>
+        <v>3324</v>
       </c>
     </row>
     <row r="1564" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -23460,7 +23463,7 @@
         <v>1562</v>
       </c>
       <c r="B1564" s="1" t="s">
-        <v>3341</v>
+        <v>3338</v>
       </c>
     </row>
     <row r="1565" spans="1:4" ht="60" x14ac:dyDescent="0.25">
@@ -23468,7 +23471,7 @@
         <v>1563</v>
       </c>
       <c r="B1565" s="1" t="s">
-        <v>3341</v>
+        <v>3338</v>
       </c>
     </row>
     <row r="1566" spans="1:4" ht="105" x14ac:dyDescent="0.25">
@@ -23476,7 +23479,7 @@
         <v>1564</v>
       </c>
       <c r="B1566" s="1" t="s">
-        <v>3342</v>
+        <v>3339</v>
       </c>
     </row>
     <row r="1567" spans="1:4" ht="135" x14ac:dyDescent="0.25">
@@ -23484,7 +23487,7 @@
         <v>1565</v>
       </c>
       <c r="B1567" s="1" t="s">
-        <v>3343</v>
+        <v>3340</v>
       </c>
     </row>
     <row r="1568" spans="1:4" ht="90" x14ac:dyDescent="0.25">
@@ -23492,10 +23495,10 @@
         <v>1566</v>
       </c>
       <c r="B1568" s="1" t="s">
-        <v>3344</v>
+        <v>3341</v>
       </c>
       <c r="C1568" s="1" t="s">
-        <v>3345</v>
+        <v>3342</v>
       </c>
     </row>
     <row r="1569" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -23503,10 +23506,10 @@
         <v>1567</v>
       </c>
       <c r="B1569" s="1" t="s">
-        <v>3346</v>
+        <v>3343</v>
       </c>
       <c r="C1569" s="1" t="s">
-        <v>3347</v>
+        <v>3344</v>
       </c>
     </row>
     <row r="1570" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23514,10 +23517,10 @@
         <v>1568</v>
       </c>
       <c r="B1570" s="1" t="s">
-        <v>3348</v>
+        <v>3345</v>
       </c>
       <c r="C1570" s="1" t="s">
-        <v>3349</v>
+        <v>3346</v>
       </c>
     </row>
     <row r="1571" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23525,10 +23528,10 @@
         <v>1569</v>
       </c>
       <c r="B1571" s="1" t="s">
-        <v>3350</v>
+        <v>3347</v>
       </c>
       <c r="C1571" s="1" t="s">
-        <v>3351</v>
+        <v>3348</v>
       </c>
     </row>
     <row r="1572" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -23536,7 +23539,7 @@
         <v>1570</v>
       </c>
       <c r="B1572" s="1" t="s">
-        <v>3352</v>
+        <v>3349</v>
       </c>
     </row>
     <row r="1573" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -23544,7 +23547,7 @@
         <v>1571</v>
       </c>
       <c r="B1573" s="1" t="s">
-        <v>3353</v>
+        <v>3350</v>
       </c>
     </row>
     <row r="1574" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -23552,7 +23555,7 @@
         <v>1572</v>
       </c>
       <c r="B1574" s="1" t="s">
-        <v>3354</v>
+        <v>3351</v>
       </c>
     </row>
     <row r="1575" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -23560,7 +23563,7 @@
         <v>1573</v>
       </c>
       <c r="B1575" s="1" t="s">
-        <v>3354</v>
+        <v>3351</v>
       </c>
     </row>
     <row r="1576" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -23568,10 +23571,10 @@
         <v>1574</v>
       </c>
       <c r="B1576" s="1" t="s">
-        <v>3355</v>
+        <v>3352</v>
       </c>
       <c r="C1576" s="1" t="s">
-        <v>3356</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="1577" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -23579,10 +23582,10 @@
         <v>1575</v>
       </c>
       <c r="B1577" s="1" t="s">
-        <v>3355</v>
+        <v>3352</v>
       </c>
       <c r="C1577" s="1" t="s">
-        <v>3356</v>
+        <v>3353</v>
       </c>
     </row>
     <row r="1578" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -23590,10 +23593,10 @@
         <v>1576</v>
       </c>
       <c r="B1578" s="1" t="s">
-        <v>3368</v>
+        <v>3365</v>
       </c>
       <c r="C1578" s="1" t="s">
-        <v>3369</v>
+        <v>3366</v>
       </c>
     </row>
     <row r="1579" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -23601,7 +23604,7 @@
         <v>1577</v>
       </c>
       <c r="B1579" s="1" t="s">
-        <v>3370</v>
+        <v>3367</v>
       </c>
     </row>
     <row r="1580" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23609,7 +23612,7 @@
         <v>1579</v>
       </c>
       <c r="B1580" s="1" t="s">
-        <v>3371</v>
+        <v>3368</v>
       </c>
     </row>
     <row r="1581" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -23617,7 +23620,7 @@
         <v>1580</v>
       </c>
       <c r="B1581" s="1" t="s">
-        <v>3372</v>
+        <v>3369</v>
       </c>
     </row>
     <row r="1582" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -23625,10 +23628,10 @@
         <v>1581</v>
       </c>
       <c r="B1582" s="1" t="s">
-        <v>3374</v>
+        <v>3371</v>
       </c>
       <c r="C1582" s="1" t="s">
-        <v>3373</v>
+        <v>3370</v>
       </c>
     </row>
     <row r="1583" spans="1:3" ht="90" x14ac:dyDescent="0.25">
@@ -23636,10 +23639,10 @@
         <v>1582</v>
       </c>
       <c r="B1583" s="1" t="s">
-        <v>3374</v>
+        <v>3371</v>
       </c>
       <c r="C1583" s="1" t="s">
-        <v>3373</v>
+        <v>3370</v>
       </c>
     </row>
     <row r="1584" spans="1:3" ht="75" x14ac:dyDescent="0.25">
@@ -23647,10 +23650,10 @@
         <v>1583</v>
       </c>
       <c r="B1584" s="1" t="s">
-        <v>3375</v>
+        <v>3372</v>
       </c>
       <c r="C1584" s="1" t="s">
-        <v>3376</v>
+        <v>3373</v>
       </c>
     </row>
     <row r="1585" spans="1:3" ht="60" x14ac:dyDescent="0.25">
@@ -23658,7 +23661,7 @@
         <v>1584</v>
       </c>
       <c r="B1585" s="1" t="s">
-        <v>3377</v>
+        <v>3374</v>
       </c>
     </row>
     <row r="1586" spans="1:3" ht="45" x14ac:dyDescent="0.25">
@@ -23666,7 +23669,7 @@
         <v>1585</v>
       </c>
       <c r="B1586" s="1" t="s">
-        <v>3378</v>
+        <v>3375</v>
       </c>
     </row>
     <row r="1587" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -23674,23 +23677,23 @@
         <v>1586</v>
       </c>
       <c r="B1587" s="1" t="s">
-        <v>3379</v>
+        <v>3376</v>
       </c>
     </row>
     <row r="1588" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A1588" s="2" t="s">
-        <v>2855</v>
+        <v>2854</v>
       </c>
       <c r="B1588" s="1" t="s">
-        <v>3380</v>
+        <v>3377</v>
       </c>
     </row>
     <row r="1589" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A1589" s="2" t="s">
-        <v>2856</v>
+        <v>2855</v>
       </c>
       <c r="B1589" s="1" t="s">
-        <v>3381</v>
+        <v>3378</v>
       </c>
     </row>
     <row r="1590" spans="1:3" x14ac:dyDescent="0.25">
@@ -23698,7 +23701,7 @@
         <v>1589</v>
       </c>
       <c r="B1590" s="1" t="s">
-        <v>3382</v>
+        <v>3379</v>
       </c>
     </row>
     <row r="1591" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -23706,74 +23709,74 @@
         <v>1588</v>
       </c>
       <c r="B1591" s="1" t="s">
-        <v>3383</v>
+        <v>3380</v>
       </c>
     </row>
     <row r="1592" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A1592" s="2" t="s">
-        <v>2857</v>
+        <v>2856</v>
       </c>
       <c r="B1592" s="1" t="s">
-        <v>3384</v>
+        <v>3381</v>
       </c>
     </row>
     <row r="1593" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A1593" s="2" t="s">
-        <v>2858</v>
+        <v>2857</v>
       </c>
       <c r="B1593" s="1" t="s">
-        <v>3385</v>
+        <v>3382</v>
       </c>
       <c r="C1593" s="1" t="s">
-        <v>3386</v>
+        <v>3383</v>
       </c>
     </row>
     <row r="1594" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A1594" s="2" t="s">
+        <v>2859</v>
+      </c>
+      <c r="B1594" s="1" t="s">
+        <v>3384</v>
+      </c>
+    </row>
+    <row r="1595" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1595" s="2" t="s">
         <v>2860</v>
       </c>
-      <c r="B1594" s="1" t="s">
-        <v>3387</v>
-      </c>
-    </row>
-    <row r="1595" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1595" s="2" t="s">
+      <c r="B1595" s="1" t="s">
+        <v>3385</v>
+      </c>
+    </row>
+    <row r="1596" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A1596" s="2" t="s">
         <v>2861</v>
       </c>
-      <c r="B1595" s="1" t="s">
-        <v>2861</v>
-      </c>
-    </row>
-    <row r="1596" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1596" s="2" t="s">
-        <v>2862</v>
-      </c>
       <c r="B1596" s="1" t="s">
-        <v>2862</v>
-      </c>
-    </row>
-    <row r="1597" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3386</v>
+      </c>
+    </row>
+    <row r="1597" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A1597" s="2" t="s">
         <v>1587</v>
       </c>
       <c r="B1597" s="1" t="s">
-        <v>1587</v>
-      </c>
-    </row>
-    <row r="1598" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3387</v>
+      </c>
+    </row>
+    <row r="1598" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A1598" s="2" t="s">
-        <v>1590</v>
+        <v>2862</v>
       </c>
       <c r="B1598" s="1" t="s">
-        <v>1590</v>
+        <v>3388</v>
       </c>
     </row>
     <row r="1599" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1599" s="2" t="s">
-        <v>2863</v>
+        <v>1590</v>
       </c>
       <c r="B1599" s="1" t="s">
-        <v>2863</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="1600" spans="1:3" x14ac:dyDescent="0.25">
@@ -23781,7 +23784,7 @@
         <v>1591</v>
       </c>
       <c r="B1600" s="1" t="s">
-        <v>3199</v>
+        <v>1591</v>
       </c>
     </row>
     <row r="1601" spans="1:2" x14ac:dyDescent="0.25">
@@ -23821,7 +23824,7 @@
         <v>1596</v>
       </c>
       <c r="B1605" s="1" t="s">
-        <v>1596</v>
+        <v>3195</v>
       </c>
     </row>
     <row r="1606" spans="1:2" x14ac:dyDescent="0.25">
@@ -23829,7 +23832,7 @@
         <v>1597</v>
       </c>
       <c r="B1606" s="1" t="s">
-        <v>3198</v>
+        <v>1597</v>
       </c>
     </row>
     <row r="1607" spans="1:2" x14ac:dyDescent="0.25">
@@ -23909,7 +23912,7 @@
         <v>1607</v>
       </c>
       <c r="B1616" s="1" t="s">
-        <v>1607</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="1617" spans="1:2" x14ac:dyDescent="0.25">
@@ -23917,7 +23920,7 @@
         <v>1608</v>
       </c>
       <c r="B1617" s="1" t="s">
-        <v>3199</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="1618" spans="1:2" x14ac:dyDescent="0.25">
@@ -23925,7 +23928,7 @@
         <v>1609</v>
       </c>
       <c r="B1618" s="1" t="s">
-        <v>3199</v>
+        <v>3196</v>
       </c>
     </row>
     <row r="1619" spans="1:2" x14ac:dyDescent="0.25">
@@ -23933,7 +23936,7 @@
         <v>1610</v>
       </c>
       <c r="B1619" s="1" t="s">
-        <v>3199</v>
+        <v>1610</v>
       </c>
     </row>
     <row r="1620" spans="1:2" x14ac:dyDescent="0.25">
@@ -23952,12 +23955,12 @@
         <v>1612</v>
       </c>
     </row>
-    <row r="1622" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1622" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1622" s="2" t="s">
         <v>1613</v>
       </c>
       <c r="B1622" s="1" t="s">
-        <v>1613</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="1623" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -23965,7 +23968,7 @@
         <v>1614</v>
       </c>
       <c r="B1623" s="1" t="s">
-        <v>3226</v>
+        <v>3223</v>
       </c>
     </row>
     <row r="1624" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -23973,15 +23976,15 @@
         <v>1615</v>
       </c>
       <c r="B1624" s="1" t="s">
-        <v>3226</v>
-      </c>
-    </row>
-    <row r="1625" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3223</v>
+      </c>
+    </row>
+    <row r="1625" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1625" s="2" t="s">
         <v>1616</v>
       </c>
       <c r="B1625" s="1" t="s">
-        <v>3226</v>
+        <v>1616</v>
       </c>
     </row>
     <row r="1626" spans="1:2" x14ac:dyDescent="0.25">
@@ -24057,11 +24060,11 @@
       </c>
     </row>
     <row r="1635" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1635" s="2" t="s">
+      <c r="A1635" s="1" t="s">
         <v>1626</v>
       </c>
       <c r="B1635" s="1" t="s">
-        <v>1626</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1636" spans="1:2" x14ac:dyDescent="0.25">
@@ -24069,7 +24072,7 @@
         <v>1627</v>
       </c>
       <c r="B1636" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1637" spans="1:2" x14ac:dyDescent="0.25">
@@ -24077,7 +24080,7 @@
         <v>1628</v>
       </c>
       <c r="B1637" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1638" spans="1:2" x14ac:dyDescent="0.25">
@@ -24085,23 +24088,23 @@
         <v>1629</v>
       </c>
       <c r="B1638" s="1" t="s">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="1639" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="1639" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1639" s="1" t="s">
         <v>1630</v>
       </c>
       <c r="B1639" s="1" t="s">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="1640" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="1640" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1640" s="1" t="s">
         <v>1631</v>
       </c>
       <c r="B1640" s="1" t="s">
-        <v>3218</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1641" spans="1:2" x14ac:dyDescent="0.25">
@@ -24109,7 +24112,7 @@
         <v>1632</v>
       </c>
       <c r="B1641" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1642" spans="1:2" x14ac:dyDescent="0.25">
@@ -24117,7 +24120,7 @@
         <v>1633</v>
       </c>
       <c r="B1642" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1643" spans="1:2" x14ac:dyDescent="0.25">
@@ -24125,7 +24128,7 @@
         <v>1634</v>
       </c>
       <c r="B1643" s="1" t="s">
-        <v>3217</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1644" spans="1:2" x14ac:dyDescent="0.25">
@@ -24133,31 +24136,31 @@
         <v>1635</v>
       </c>
       <c r="B1644" s="1" t="s">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="1645" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3214</v>
+      </c>
+    </row>
+    <row r="1645" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1645" s="1" t="s">
         <v>1636</v>
       </c>
       <c r="B1645" s="1" t="s">
-        <v>3217</v>
-      </c>
-    </row>
-    <row r="1646" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3215</v>
+      </c>
+    </row>
+    <row r="1646" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1646" s="1" t="s">
         <v>1637</v>
       </c>
       <c r="B1646" s="1" t="s">
-        <v>3218</v>
+        <v>3214</v>
       </c>
     </row>
     <row r="1647" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1647" s="1" t="s">
+      <c r="A1647" s="2" t="s">
         <v>1638</v>
       </c>
       <c r="B1647" s="1" t="s">
-        <v>3217</v>
+        <v>1638</v>
       </c>
     </row>
     <row r="1648" spans="1:2" x14ac:dyDescent="0.25">
@@ -24181,10 +24184,10 @@
         <v>1641</v>
       </c>
       <c r="B1650" s="1" t="s">
-        <v>1641</v>
-      </c>
-    </row>
-    <row r="1651" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3207</v>
+      </c>
+    </row>
+    <row r="1651" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1651" s="2" t="s">
         <v>1642</v>
       </c>
@@ -24192,20 +24195,20 @@
         <v>3210</v>
       </c>
     </row>
-    <row r="1652" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="1652" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1652" s="2" t="s">
         <v>1643</v>
       </c>
       <c r="B1652" s="1" t="s">
-        <v>3213</v>
-      </c>
-    </row>
-    <row r="1653" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="1653" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1653" s="2" t="s">
         <v>1644</v>
       </c>
       <c r="B1653" s="1" t="s">
-        <v>3212</v>
+        <v>1644</v>
       </c>
     </row>
     <row r="1654" spans="1:2" x14ac:dyDescent="0.25">
@@ -24229,31 +24232,31 @@
         <v>1647</v>
       </c>
       <c r="B1656" s="1" t="s">
-        <v>1647</v>
-      </c>
-    </row>
-    <row r="1657" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3208</v>
+      </c>
+    </row>
+    <row r="1657" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1657" s="2" t="s">
         <v>1648</v>
       </c>
       <c r="B1657" s="1" t="s">
-        <v>3211</v>
-      </c>
-    </row>
-    <row r="1658" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3210</v>
+      </c>
+    </row>
+    <row r="1658" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1658" s="2" t="s">
         <v>1649</v>
       </c>
       <c r="B1658" s="1" t="s">
-        <v>3213</v>
-      </c>
-    </row>
-    <row r="1659" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3209</v>
+      </c>
+    </row>
+    <row r="1659" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1659" s="2" t="s">
         <v>1650</v>
       </c>
       <c r="B1659" s="1" t="s">
-        <v>3212</v>
+        <v>1650</v>
       </c>
     </row>
     <row r="1660" spans="1:2" x14ac:dyDescent="0.25">
@@ -24264,20 +24267,20 @@
         <v>1651</v>
       </c>
     </row>
-    <row r="1661" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1661" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1661" s="2" t="s">
         <v>1652</v>
       </c>
       <c r="B1661" s="1" t="s">
-        <v>1652</v>
-      </c>
-    </row>
-    <row r="1662" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="1662" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1662" s="2" t="s">
         <v>1653</v>
       </c>
       <c r="B1662" s="1" t="s">
-        <v>3209</v>
+        <v>1653</v>
       </c>
     </row>
     <row r="1663" spans="1:2" x14ac:dyDescent="0.25">
@@ -24312,20 +24315,20 @@
         <v>1657</v>
       </c>
     </row>
-    <row r="1667" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1667" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1667" s="2" t="s">
         <v>1658</v>
       </c>
       <c r="B1667" s="1" t="s">
-        <v>1658</v>
-      </c>
-    </row>
-    <row r="1668" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3206</v>
+      </c>
+    </row>
+    <row r="1668" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1668" s="2" t="s">
         <v>1659</v>
       </c>
       <c r="B1668" s="1" t="s">
-        <v>3209</v>
+        <v>1659</v>
       </c>
     </row>
     <row r="1669" spans="1:2" x14ac:dyDescent="0.25">
@@ -24349,39 +24352,39 @@
         <v>1662</v>
       </c>
       <c r="B1671" s="1" t="s">
-        <v>1662</v>
-      </c>
-    </row>
-    <row r="1672" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1672" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1672" s="2" t="s">
         <v>1663</v>
       </c>
       <c r="B1672" s="1" t="s">
-        <v>3232</v>
-      </c>
-    </row>
-    <row r="1673" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="1673" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1673" s="2" t="s">
         <v>1664</v>
       </c>
       <c r="B1673" s="1" t="s">
-        <v>3234</v>
-      </c>
-    </row>
-    <row r="1674" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1674" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1674" s="2" t="s">
         <v>1665</v>
       </c>
       <c r="B1674" s="1" t="s">
-        <v>3232</v>
-      </c>
-    </row>
-    <row r="1675" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="1675" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1675" s="2" t="s">
         <v>1666</v>
       </c>
       <c r="B1675" s="1" t="s">
-        <v>3234</v>
+        <v>3229</v>
       </c>
     </row>
     <row r="1676" spans="1:2" x14ac:dyDescent="0.25">
@@ -24389,55 +24392,55 @@
         <v>1667</v>
       </c>
       <c r="B1676" s="1" t="s">
-        <v>3232</v>
-      </c>
-    </row>
-    <row r="1677" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1677" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1677" s="2" t="s">
         <v>1668</v>
       </c>
       <c r="B1677" s="1" t="s">
-        <v>3232</v>
-      </c>
-    </row>
-    <row r="1678" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="1678" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1678" s="2" t="s">
         <v>1669</v>
       </c>
       <c r="B1678" s="1" t="s">
-        <v>3234</v>
-      </c>
-    </row>
-    <row r="1679" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1679" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1679" s="2" t="s">
         <v>1670</v>
       </c>
       <c r="B1679" s="1" t="s">
-        <v>3232</v>
-      </c>
-    </row>
-    <row r="1680" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3231</v>
+      </c>
+    </row>
+    <row r="1680" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1680" s="2" t="s">
         <v>1671</v>
       </c>
       <c r="B1680" s="1" t="s">
-        <v>3234</v>
-      </c>
-    </row>
-    <row r="1681" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3229</v>
+      </c>
+    </row>
+    <row r="1681" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1681" s="2" t="s">
         <v>1672</v>
       </c>
       <c r="B1681" s="1" t="s">
-        <v>3232</v>
-      </c>
-    </row>
-    <row r="1682" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3230</v>
+      </c>
+    </row>
+    <row r="1682" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1682" s="2" t="s">
         <v>1673</v>
       </c>
       <c r="B1682" s="1" t="s">
-        <v>3233</v>
+        <v>1673</v>
       </c>
     </row>
     <row r="1683" spans="1:2" x14ac:dyDescent="0.25">
@@ -24504,12 +24507,12 @@
         <v>1681</v>
       </c>
     </row>
-    <row r="1691" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1691" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1691" s="2" t="s">
         <v>1682</v>
       </c>
       <c r="B1691" s="1" t="s">
-        <v>1682</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="1692" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24517,7 +24520,7 @@
         <v>1683</v>
       </c>
       <c r="B1692" s="1" t="s">
-        <v>3236</v>
+        <v>3233</v>
       </c>
     </row>
     <row r="1693" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24525,23 +24528,23 @@
         <v>1684</v>
       </c>
       <c r="B1693" s="1" t="s">
-        <v>3236</v>
-      </c>
-    </row>
-    <row r="1694" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3233</v>
+      </c>
+    </row>
+    <row r="1694" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1694" s="2" t="s">
         <v>1685</v>
       </c>
       <c r="B1694" s="1" t="s">
-        <v>3236</v>
-      </c>
-    </row>
-    <row r="1695" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="1695" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1695" s="2" t="s">
         <v>1686</v>
       </c>
       <c r="B1695" s="1" t="s">
-        <v>3241</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="1696" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24549,7 +24552,7 @@
         <v>1687</v>
       </c>
       <c r="B1696" s="1" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="1697" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24557,7 +24560,7 @@
         <v>1688</v>
       </c>
       <c r="B1697" s="1" t="s">
-        <v>3240</v>
+        <v>3234</v>
       </c>
     </row>
     <row r="1698" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24565,7 +24568,7 @@
         <v>1689</v>
       </c>
       <c r="B1698" s="1" t="s">
-        <v>3237</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="1699" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24573,23 +24576,23 @@
         <v>1690</v>
       </c>
       <c r="B1699" s="1" t="s">
-        <v>3239</v>
-      </c>
-    </row>
-    <row r="1700" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3234</v>
+      </c>
+    </row>
+    <row r="1700" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1700" s="2" t="s">
         <v>1691</v>
       </c>
       <c r="B1700" s="1" t="s">
-        <v>3237</v>
-      </c>
-    </row>
-    <row r="1701" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3238</v>
+      </c>
+    </row>
+    <row r="1701" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1701" s="2" t="s">
         <v>1692</v>
       </c>
       <c r="B1701" s="1" t="s">
-        <v>3241</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="1702" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24597,7 +24600,7 @@
         <v>1693</v>
       </c>
       <c r="B1702" s="1" t="s">
-        <v>3238</v>
+        <v>3237</v>
       </c>
     </row>
     <row r="1703" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24605,7 +24608,7 @@
         <v>1694</v>
       </c>
       <c r="B1703" s="1" t="s">
-        <v>3240</v>
+        <v>3235</v>
       </c>
     </row>
     <row r="1704" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24613,7 +24616,7 @@
         <v>1695</v>
       </c>
       <c r="B1704" s="1" t="s">
-        <v>3238</v>
+        <v>3236</v>
       </c>
     </row>
     <row r="1705" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24621,23 +24624,23 @@
         <v>1696</v>
       </c>
       <c r="B1705" s="1" t="s">
-        <v>3239</v>
-      </c>
-    </row>
-    <row r="1706" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3235</v>
+      </c>
+    </row>
+    <row r="1706" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1706" s="2" t="s">
         <v>1697</v>
       </c>
       <c r="B1706" s="1" t="s">
-        <v>3238</v>
-      </c>
-    </row>
-    <row r="1707" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="1707" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1707" s="2" t="s">
         <v>1698</v>
       </c>
       <c r="B1707" s="1" t="s">
-        <v>3243</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="1708" spans="1:2" x14ac:dyDescent="0.25">
@@ -24645,7 +24648,7 @@
         <v>1699</v>
       </c>
       <c r="B1708" s="1" t="s">
-        <v>3242</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="1709" spans="1:2" x14ac:dyDescent="0.25">
@@ -24653,10 +24656,10 @@
         <v>1700</v>
       </c>
       <c r="B1709" s="1" t="s">
-        <v>3242</v>
-      </c>
-    </row>
-    <row r="1710" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="1710" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1710" s="2" t="s">
         <v>1701</v>
       </c>
@@ -24669,7 +24672,7 @@
         <v>1702</v>
       </c>
       <c r="B1711" s="1" t="s">
-        <v>3245</v>
+        <v>3241</v>
       </c>
     </row>
     <row r="1712" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -24677,15 +24680,15 @@
         <v>1703</v>
       </c>
       <c r="B1712" s="1" t="s">
-        <v>3244</v>
-      </c>
-    </row>
-    <row r="1713" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="1713" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1713" s="2" t="s">
         <v>1704</v>
       </c>
       <c r="B1713" s="1" t="s">
-        <v>3243</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="1714" spans="1:2" x14ac:dyDescent="0.25">
@@ -24693,7 +24696,7 @@
         <v>1705</v>
       </c>
       <c r="B1714" s="1" t="s">
-        <v>3242</v>
+        <v>3239</v>
       </c>
     </row>
     <row r="1715" spans="1:2" x14ac:dyDescent="0.25">
@@ -24701,10 +24704,10 @@
         <v>1706</v>
       </c>
       <c r="B1715" s="1" t="s">
-        <v>3242</v>
-      </c>
-    </row>
-    <row r="1716" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3239</v>
+      </c>
+    </row>
+    <row r="1716" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1716" s="2" t="s">
         <v>1707</v>
       </c>
@@ -24717,15 +24720,15 @@
         <v>1708</v>
       </c>
       <c r="B1717" s="1" t="s">
-        <v>3245</v>
-      </c>
-    </row>
-    <row r="1718" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3240</v>
+      </c>
+    </row>
+    <row r="1718" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1718" s="2" t="s">
         <v>1709</v>
       </c>
       <c r="B1718" s="1" t="s">
-        <v>3243</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="1719" spans="1:2" x14ac:dyDescent="0.25">
@@ -24733,7 +24736,7 @@
         <v>1710</v>
       </c>
       <c r="B1719" s="1" t="s">
-        <v>1710</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="1720" spans="1:2" x14ac:dyDescent="0.25">
@@ -24741,23 +24744,23 @@
         <v>1711</v>
       </c>
       <c r="B1720" s="1" t="s">
-        <v>3251</v>
-      </c>
-    </row>
-    <row r="1721" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="1721" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1721" s="2" t="s">
         <v>1712</v>
       </c>
       <c r="B1721" s="1" t="s">
-        <v>1712</v>
-      </c>
-    </row>
-    <row r="1722" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3249</v>
+      </c>
+    </row>
+    <row r="1722" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1722" s="2" t="s">
         <v>1713</v>
       </c>
       <c r="B1722" s="1" t="s">
-        <v>3252</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="1723" spans="1:2" x14ac:dyDescent="0.25">
@@ -24765,7 +24768,7 @@
         <v>1714</v>
       </c>
       <c r="B1723" s="1" t="s">
-        <v>1714</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="1724" spans="1:2" x14ac:dyDescent="0.25">
@@ -24773,7 +24776,7 @@
         <v>1715</v>
       </c>
       <c r="B1724" s="1" t="s">
-        <v>3251</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="1725" spans="1:2" x14ac:dyDescent="0.25">
@@ -24781,7 +24784,7 @@
         <v>1716</v>
       </c>
       <c r="B1725" s="1" t="s">
-        <v>1716</v>
+        <v>3248</v>
       </c>
     </row>
     <row r="1726" spans="1:2" x14ac:dyDescent="0.25">
@@ -24789,7 +24792,7 @@
         <v>1717</v>
       </c>
       <c r="B1726" s="1" t="s">
-        <v>3251</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="1727" spans="1:2" x14ac:dyDescent="0.25">
@@ -24805,23 +24808,23 @@
         <v>1719</v>
       </c>
       <c r="B1728" s="1" t="s">
-        <v>1719</v>
-      </c>
-    </row>
-    <row r="1729" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3248</v>
+      </c>
+    </row>
+    <row r="1729" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1729" s="2" t="s">
         <v>1720</v>
       </c>
       <c r="B1729" s="1" t="s">
-        <v>3251</v>
-      </c>
-    </row>
-    <row r="1730" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="1730" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1730" s="2" t="s">
         <v>1721</v>
       </c>
       <c r="B1730" s="1" t="s">
-        <v>3255</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="1731" spans="1:2" x14ac:dyDescent="0.25">
@@ -24829,7 +24832,7 @@
         <v>1722</v>
       </c>
       <c r="B1731" s="1" t="s">
-        <v>3254</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1732" spans="1:2" x14ac:dyDescent="0.25">
@@ -24853,7 +24856,7 @@
         <v>1725</v>
       </c>
       <c r="B1734" s="1" t="s">
-        <v>1725</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="1735" spans="1:2" x14ac:dyDescent="0.25">
@@ -24861,7 +24864,7 @@
         <v>1726</v>
       </c>
       <c r="B1735" s="1" t="s">
-        <v>3253</v>
+        <v>3250</v>
       </c>
     </row>
     <row r="1736" spans="1:2" x14ac:dyDescent="0.25">
@@ -24869,7 +24872,7 @@
         <v>1727</v>
       </c>
       <c r="B1736" s="1" t="s">
-        <v>3253</v>
+        <v>3251</v>
       </c>
     </row>
     <row r="1737" spans="1:2" x14ac:dyDescent="0.25">
@@ -24877,7 +24880,7 @@
         <v>1728</v>
       </c>
       <c r="B1737" s="1" t="s">
-        <v>3254</v>
+        <v>1728</v>
       </c>
     </row>
     <row r="1738" spans="1:2" x14ac:dyDescent="0.25">
@@ -24896,20 +24899,20 @@
         <v>1730</v>
       </c>
     </row>
-    <row r="1740" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1740" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A1740" s="2" t="s">
         <v>1731</v>
       </c>
       <c r="B1740" s="1" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="1741" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3252</v>
+      </c>
+    </row>
+    <row r="1741" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1741" s="2" t="s">
         <v>1732</v>
       </c>
       <c r="B1741" s="1" t="s">
-        <v>3255</v>
+        <v>1732</v>
       </c>
     </row>
     <row r="1742" spans="1:2" x14ac:dyDescent="0.25">
@@ -24925,7 +24928,7 @@
         <v>1734</v>
       </c>
       <c r="B1743" s="1" t="s">
-        <v>1734</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="1744" spans="1:2" x14ac:dyDescent="0.25">
@@ -24933,23 +24936,23 @@
         <v>1735</v>
       </c>
       <c r="B1744" s="1" t="s">
-        <v>3258</v>
-      </c>
-    </row>
-    <row r="1745" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1735</v>
+      </c>
+    </row>
+    <row r="1745" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1745" s="2" t="s">
         <v>1736</v>
       </c>
       <c r="B1745" s="1" t="s">
-        <v>1736</v>
-      </c>
-    </row>
-    <row r="1746" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="1746" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1746" s="2" t="s">
         <v>1737</v>
       </c>
       <c r="B1746" s="1" t="s">
-        <v>3260</v>
+        <v>3256</v>
       </c>
     </row>
     <row r="1747" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -24957,15 +24960,15 @@
         <v>1738</v>
       </c>
       <c r="B1747" s="1" t="s">
-        <v>3259</v>
-      </c>
-    </row>
-    <row r="1748" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3256</v>
+      </c>
+    </row>
+    <row r="1748" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1748" s="2" t="s">
         <v>1739</v>
       </c>
       <c r="B1748" s="1" t="s">
-        <v>3259</v>
+        <v>1739</v>
       </c>
     </row>
     <row r="1749" spans="1:2" x14ac:dyDescent="0.25">
@@ -24973,7 +24976,7 @@
         <v>1740</v>
       </c>
       <c r="B1749" s="1" t="s">
-        <v>1740</v>
+        <v>3255</v>
       </c>
     </row>
     <row r="1750" spans="1:2" x14ac:dyDescent="0.25">
@@ -24981,23 +24984,23 @@
         <v>1741</v>
       </c>
       <c r="B1750" s="1" t="s">
-        <v>3258</v>
-      </c>
-    </row>
-    <row r="1751" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1741</v>
+      </c>
+    </row>
+    <row r="1751" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1751" s="2" t="s">
         <v>1742</v>
       </c>
       <c r="B1751" s="1" t="s">
-        <v>1742</v>
-      </c>
-    </row>
-    <row r="1752" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>3257</v>
+      </c>
+    </row>
+    <row r="1752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1752" s="2" t="s">
         <v>1743</v>
       </c>
       <c r="B1752" s="1" t="s">
-        <v>3260</v>
+        <v>1743</v>
       </c>
     </row>
     <row r="1753" spans="1:2" x14ac:dyDescent="0.25">
@@ -25005,7 +25008,7 @@
         <v>1744</v>
       </c>
       <c r="B1753" s="1" t="s">
-        <v>1744</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="1754" spans="1:2" x14ac:dyDescent="0.25">
@@ -25013,39 +25016,39 @@
         <v>1745</v>
       </c>
       <c r="B1754" s="1" t="s">
-        <v>3263</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="1755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1755" s="2" t="s">
         <v>1746</v>
       </c>
-      <c r="B1755" s="1" t="s">
-        <v>1746</v>
+      <c r="B1755" s="3" t="s">
+        <v>3261</v>
       </c>
     </row>
     <row r="1756" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1756" s="2" t="s">
         <v>1747</v>
       </c>
-      <c r="B1756" s="3" t="s">
-        <v>3264</v>
+      <c r="B1756" s="1" t="s">
+        <v>1747</v>
       </c>
     </row>
     <row r="1757" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1757" s="2" t="s">
         <v>1748</v>
       </c>
-      <c r="B1757" s="1" t="s">
-        <v>1748</v>
+      <c r="B1757" s="3" t="s">
+        <v>3262</v>
       </c>
     </row>
     <row r="1758" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1758" s="2" t="s">
         <v>1749</v>
       </c>
-      <c r="B1758" s="3" t="s">
-        <v>3265</v>
+      <c r="B1758" s="1" t="s">
+        <v>1749</v>
       </c>
     </row>
     <row r="1759" spans="1:2" x14ac:dyDescent="0.25">
@@ -25053,7 +25056,7 @@
         <v>1750</v>
       </c>
       <c r="B1759" s="1" t="s">
-        <v>1750</v>
+        <v>3260</v>
       </c>
     </row>
     <row r="1760" spans="1:2" x14ac:dyDescent="0.25">
@@ -25061,39 +25064,39 @@
         <v>1751</v>
       </c>
       <c r="B1760" s="1" t="s">
-        <v>3263</v>
+        <v>1751</v>
       </c>
     </row>
     <row r="1761" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1761" s="2" t="s">
         <v>1752</v>
       </c>
-      <c r="B1761" s="1" t="s">
-        <v>1752</v>
+      <c r="B1761" s="3" t="s">
+        <v>3261</v>
       </c>
     </row>
     <row r="1762" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1762" s="2" t="s">
         <v>1753</v>
       </c>
-      <c r="B1762" s="3" t="s">
-        <v>3264</v>
+      <c r="B1762" s="1" t="s">
+        <v>1753</v>
       </c>
     </row>
     <row r="1763" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1763" s="2" t="s">
         <v>1754</v>
       </c>
-      <c r="B1763" s="1" t="s">
-        <v>1754</v>
+      <c r="B1763" s="3" t="s">
+        <v>3262</v>
       </c>
     </row>
     <row r="1764" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1764" s="2" t="s">
         <v>1755</v>
       </c>
-      <c r="B1764" s="3" t="s">
-        <v>3265</v>
+      <c r="B1764" s="1" t="s">
+        <v>1755</v>
       </c>
     </row>
     <row r="1765" spans="1:2" x14ac:dyDescent="0.25">
@@ -25576,12 +25579,12 @@
         <v>1815</v>
       </c>
     </row>
-    <row r="1825" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1825" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1825" s="2" t="s">
         <v>1816</v>
       </c>
       <c r="B1825" s="1" t="s">
-        <v>1816</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1826" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25589,7 +25592,7 @@
         <v>1817</v>
       </c>
       <c r="B1826" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1827" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25597,7 +25600,7 @@
         <v>1818</v>
       </c>
       <c r="B1827" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1828" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25605,7 +25608,7 @@
         <v>1819</v>
       </c>
       <c r="B1828" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1829" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25613,7 +25616,7 @@
         <v>1820</v>
       </c>
       <c r="B1829" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1830" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25621,7 +25624,7 @@
         <v>1821</v>
       </c>
       <c r="B1830" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1831" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25629,7 +25632,7 @@
         <v>1822</v>
       </c>
       <c r="B1831" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1832" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25637,7 +25640,7 @@
         <v>1823</v>
       </c>
       <c r="B1832" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1833" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25645,7 +25648,7 @@
         <v>1824</v>
       </c>
       <c r="B1833" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1834" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25653,7 +25656,7 @@
         <v>1825</v>
       </c>
       <c r="B1834" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1835" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25661,7 +25664,7 @@
         <v>1826</v>
       </c>
       <c r="B1835" s="1" t="s">
-        <v>3235</v>
+        <v>3232</v>
       </c>
     </row>
     <row r="1836" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -25669,15 +25672,15 @@
         <v>1827</v>
       </c>
       <c r="B1836" s="1" t="s">
-        <v>3235</v>
-      </c>
-    </row>
-    <row r="1837" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3232</v>
+      </c>
+    </row>
+    <row r="1837" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1837" s="2" t="s">
         <v>1828</v>
       </c>
       <c r="B1837" s="1" t="s">
-        <v>3235</v>
+        <v>1828</v>
       </c>
     </row>
     <row r="1838" spans="1:2" x14ac:dyDescent="0.25">
@@ -28264,20 +28267,20 @@
         <v>2151</v>
       </c>
     </row>
-    <row r="2161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2161" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2161" s="2" t="s">
         <v>2152</v>
       </c>
       <c r="B2161" s="1" t="s">
-        <v>2152</v>
-      </c>
-    </row>
-    <row r="2162" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3243</v>
+      </c>
+    </row>
+    <row r="2162" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2162" s="2" t="s">
         <v>2153</v>
       </c>
       <c r="B2162" s="1" t="s">
-        <v>3246</v>
+        <v>2153</v>
       </c>
     </row>
     <row r="2163" spans="1:2" x14ac:dyDescent="0.25">
@@ -28312,20 +28315,20 @@
         <v>2157</v>
       </c>
     </row>
-    <row r="2167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2167" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2167" s="2" t="s">
         <v>2158</v>
       </c>
       <c r="B2167" s="1" t="s">
-        <v>2158</v>
-      </c>
-    </row>
-    <row r="2168" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3253</v>
+      </c>
+    </row>
+    <row r="2168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2168" s="2" t="s">
         <v>2159</v>
       </c>
       <c r="B2168" s="1" t="s">
-        <v>3256</v>
+        <v>2159</v>
       </c>
     </row>
     <row r="2169" spans="1:2" x14ac:dyDescent="0.25">
@@ -28529,7 +28532,7 @@
       </c>
     </row>
     <row r="2194" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2194" s="2" t="s">
+      <c r="A2194" s="1" t="s">
         <v>2185</v>
       </c>
       <c r="B2194" s="1" t="s">
@@ -29481,7 +29484,7 @@
       </c>
     </row>
     <row r="2313" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2313" s="1" t="s">
+      <c r="A2313" s="2" t="s">
         <v>2304</v>
       </c>
       <c r="B2313" s="1" t="s">
@@ -33880,12 +33883,12 @@
         <v>2853</v>
       </c>
     </row>
-    <row r="2863" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2863" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2863" s="2" t="s">
-        <v>2854</v>
+        <v>2863</v>
       </c>
       <c r="B2863" s="1" t="s">
-        <v>2854</v>
+        <v>3197</v>
       </c>
     </row>
     <row r="2864" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33893,7 +33896,7 @@
         <v>2864</v>
       </c>
       <c r="B2864" s="1" t="s">
-        <v>3200</v>
+        <v>3198</v>
       </c>
     </row>
     <row r="2865" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33901,7 +33904,7 @@
         <v>2865</v>
       </c>
       <c r="B2865" s="1" t="s">
-        <v>3201</v>
+        <v>3199</v>
       </c>
     </row>
     <row r="2866" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33909,47 +33912,47 @@
         <v>2866</v>
       </c>
       <c r="B2866" s="1" t="s">
-        <v>3202</v>
-      </c>
-    </row>
-    <row r="2867" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3200</v>
+      </c>
+    </row>
+    <row r="2867" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2867" s="2" t="s">
         <v>2867</v>
       </c>
       <c r="B2867" s="1" t="s">
-        <v>3203</v>
-      </c>
-    </row>
-    <row r="2868" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3201</v>
+      </c>
+    </row>
+    <row r="2868" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2868" s="2" t="s">
         <v>2868</v>
       </c>
       <c r="B2868" s="1" t="s">
-        <v>3204</v>
-      </c>
-    </row>
-    <row r="2869" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3202</v>
+      </c>
+    </row>
+    <row r="2869" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2869" s="2" t="s">
         <v>2869</v>
       </c>
       <c r="B2869" s="1" t="s">
-        <v>3205</v>
-      </c>
-    </row>
-    <row r="2870" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3203</v>
+      </c>
+    </row>
+    <row r="2870" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2870" s="2" t="s">
         <v>2870</v>
       </c>
       <c r="B2870" s="1" t="s">
-        <v>3206</v>
-      </c>
-    </row>
-    <row r="2871" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3204</v>
+      </c>
+    </row>
+    <row r="2871" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2871" s="2" t="s">
         <v>2871</v>
       </c>
       <c r="B2871" s="1" t="s">
-        <v>3207</v>
+        <v>3205</v>
       </c>
     </row>
     <row r="2872" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33957,7 +33960,7 @@
         <v>2872</v>
       </c>
       <c r="B2872" s="1" t="s">
-        <v>3208</v>
+        <v>3211</v>
       </c>
     </row>
     <row r="2873" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33965,7 +33968,7 @@
         <v>2873</v>
       </c>
       <c r="B2873" s="1" t="s">
-        <v>3214</v>
+        <v>3212</v>
       </c>
     </row>
     <row r="2874" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -33973,39 +33976,39 @@
         <v>2874</v>
       </c>
       <c r="B2874" s="1" t="s">
-        <v>3215</v>
-      </c>
-    </row>
-    <row r="2875" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3213</v>
+      </c>
+    </row>
+    <row r="2875" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2875" s="2" t="s">
         <v>2875</v>
       </c>
       <c r="B2875" s="1" t="s">
-        <v>3216</v>
-      </c>
-    </row>
-    <row r="2876" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A2876" s="2" t="s">
+        <v>3245</v>
+      </c>
+    </row>
+    <row r="2876" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2876" s="1" t="s">
         <v>2876</v>
       </c>
       <c r="B2876" s="1" t="s">
-        <v>3248</v>
-      </c>
-    </row>
-    <row r="2877" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3219</v>
+      </c>
+    </row>
+    <row r="2877" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2877" s="1" t="s">
         <v>2877</v>
       </c>
       <c r="B2877" s="1" t="s">
-        <v>3222</v>
-      </c>
-    </row>
-    <row r="2878" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3218</v>
+      </c>
+    </row>
+    <row r="2878" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2878" s="1" t="s">
         <v>2878</v>
       </c>
       <c r="B2878" s="1" t="s">
-        <v>3221</v>
+        <v>3217</v>
       </c>
     </row>
     <row r="2879" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34013,15 +34016,15 @@
         <v>2879</v>
       </c>
       <c r="B2879" s="1" t="s">
-        <v>3220</v>
+        <v>3216</v>
       </c>
     </row>
     <row r="2880" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2880" s="1" t="s">
+      <c r="A2880" s="2" t="s">
         <v>2880</v>
       </c>
       <c r="B2880" s="1" t="s">
-        <v>3219</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="2881" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34029,7 +34032,7 @@
         <v>2881</v>
       </c>
       <c r="B2881" s="1" t="s">
-        <v>3225</v>
+        <v>3222</v>
       </c>
     </row>
     <row r="2882" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34045,7 +34048,7 @@
         <v>2883</v>
       </c>
       <c r="B2883" s="1" t="s">
-        <v>3228</v>
+        <v>3224</v>
       </c>
     </row>
     <row r="2884" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34053,7 +34056,7 @@
         <v>2884</v>
       </c>
       <c r="B2884" s="1" t="s">
-        <v>3227</v>
+        <v>3226</v>
       </c>
     </row>
     <row r="2885" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34061,18 +34064,18 @@
         <v>2885</v>
       </c>
       <c r="B2885" s="1" t="s">
-        <v>3229</v>
-      </c>
-    </row>
-    <row r="2886" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3227</v>
+      </c>
+    </row>
+    <row r="2886" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2886" s="2" t="s">
         <v>2886</v>
       </c>
       <c r="B2886" s="1" t="s">
-        <v>3230</v>
-      </c>
-    </row>
-    <row r="2887" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2886</v>
+      </c>
+    </row>
+    <row r="2887" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2887" s="2" t="s">
         <v>2887</v>
       </c>
@@ -34093,7 +34096,7 @@
         <v>2889</v>
       </c>
       <c r="B2889" s="1" t="s">
-        <v>2889</v>
+        <v>3265</v>
       </c>
     </row>
     <row r="2890" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34101,7 +34104,7 @@
         <v>2890</v>
       </c>
       <c r="B2890" s="1" t="s">
-        <v>3268</v>
+        <v>3266</v>
       </c>
     </row>
     <row r="2891" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -34109,15 +34112,15 @@
         <v>2891</v>
       </c>
       <c r="B2891" s="1" t="s">
-        <v>3269</v>
-      </c>
-    </row>
-    <row r="2892" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3267</v>
+      </c>
+    </row>
+    <row r="2892" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2892" s="2" t="s">
         <v>2892</v>
       </c>
       <c r="B2892" s="1" t="s">
-        <v>3270</v>
+        <v>2892</v>
       </c>
     </row>
     <row r="2893" spans="1:2" x14ac:dyDescent="0.25">
@@ -34141,7 +34144,7 @@
         <v>2895</v>
       </c>
       <c r="B2895" s="1" t="s">
-        <v>2895</v>
+        <v>3269</v>
       </c>
     </row>
     <row r="2896" spans="1:2" x14ac:dyDescent="0.25">
@@ -34149,15 +34152,15 @@
         <v>2896</v>
       </c>
       <c r="B2896" s="1" t="s">
-        <v>3272</v>
-      </c>
-    </row>
-    <row r="2897" spans="1:2" x14ac:dyDescent="0.25">
+        <v>3269</v>
+      </c>
+    </row>
+    <row r="2897" spans="1:2" ht="60" x14ac:dyDescent="0.25">
       <c r="A2897" s="2" t="s">
         <v>2897</v>
       </c>
       <c r="B2897" s="1" t="s">
-        <v>3272</v>
+        <v>3270</v>
       </c>
     </row>
     <row r="2898" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -34165,15 +34168,15 @@
         <v>2898</v>
       </c>
       <c r="B2898" s="1" t="s">
-        <v>3273</v>
-      </c>
-    </row>
-    <row r="2899" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3270</v>
+      </c>
+    </row>
+    <row r="2899" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2899" s="2" t="s">
         <v>2899</v>
       </c>
       <c r="B2899" s="1" t="s">
-        <v>3273</v>
+        <v>2899</v>
       </c>
     </row>
     <row r="2900" spans="1:2" x14ac:dyDescent="0.25">
@@ -34184,7 +34187,7 @@
         <v>2900</v>
       </c>
     </row>
-    <row r="2901" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2901" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2901" s="2" t="s">
         <v>2901</v>
       </c>
@@ -34200,23 +34203,23 @@
         <v>2902</v>
       </c>
     </row>
-    <row r="2903" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2903" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A2903" s="2" t="s">
         <v>2903</v>
       </c>
       <c r="B2903" s="1" t="s">
-        <v>2903</v>
-      </c>
-    </row>
-    <row r="2904" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>3304</v>
+      </c>
+    </row>
+    <row r="2904" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2904" s="2" t="s">
         <v>2904</v>
       </c>
       <c r="B2904" s="1" t="s">
-        <v>3307</v>
-      </c>
-    </row>
-    <row r="2905" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2904</v>
+      </c>
+    </row>
+    <row r="2905" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2905" s="2" t="s">
         <v>2905</v>
       </c>
@@ -34232,7 +34235,7 @@
         <v>2906</v>
       </c>
     </row>
-    <row r="2907" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2907" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2907" s="2" t="s">
         <v>2907</v>
       </c>
@@ -34248,7 +34251,7 @@
         <v>2908</v>
       </c>
     </row>
-    <row r="2909" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2909" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2909" s="2" t="s">
         <v>2909</v>
       </c>
@@ -34256,7 +34259,7 @@
         <v>2909</v>
       </c>
     </row>
-    <row r="2910" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2910" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2910" s="2" t="s">
         <v>2910</v>
       </c>
@@ -34576,7 +34579,7 @@
         <v>2949</v>
       </c>
     </row>
-    <row r="2950" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2950" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A2950" s="2" t="s">
         <v>2950</v>
       </c>
@@ -34584,7 +34587,7 @@
         <v>2950</v>
       </c>
     </row>
-    <row r="2951" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="2951" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2951" s="2" t="s">
         <v>2951</v>
       </c>
@@ -34664,7 +34667,7 @@
         <v>2960</v>
       </c>
     </row>
-    <row r="2961" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2961" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2961" s="2" t="s">
         <v>2961</v>
       </c>
@@ -34672,7 +34675,7 @@
         <v>2961</v>
       </c>
     </row>
-    <row r="2962" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2962" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2962" s="2" t="s">
         <v>2962</v>
       </c>
@@ -34680,7 +34683,7 @@
         <v>2962</v>
       </c>
     </row>
-    <row r="2963" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2963" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2963" s="2" t="s">
         <v>2963</v>
       </c>
@@ -34688,7 +34691,7 @@
         <v>2963</v>
       </c>
     </row>
-    <row r="2964" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2964" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2964" s="2" t="s">
         <v>2964</v>
       </c>
@@ -34696,7 +34699,7 @@
         <v>2964</v>
       </c>
     </row>
-    <row r="2965" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2965" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2965" s="2" t="s">
         <v>2965</v>
       </c>
@@ -34704,7 +34707,7 @@
         <v>2965</v>
       </c>
     </row>
-    <row r="2966" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2966" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2966" s="2" t="s">
         <v>2966</v>
       </c>
@@ -34712,7 +34715,7 @@
         <v>2966</v>
       </c>
     </row>
-    <row r="2967" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2967" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2967" s="2" t="s">
         <v>2967</v>
       </c>
@@ -34720,7 +34723,7 @@
         <v>2967</v>
       </c>
     </row>
-    <row r="2968" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2968" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2968" s="2" t="s">
         <v>2968</v>
       </c>
@@ -34728,7 +34731,7 @@
         <v>2968</v>
       </c>
     </row>
-    <row r="2969" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2969" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2969" s="2" t="s">
         <v>2969</v>
       </c>
@@ -34736,7 +34739,7 @@
         <v>2969</v>
       </c>
     </row>
-    <row r="2970" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2970" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2970" s="2" t="s">
         <v>2970</v>
       </c>
@@ -34744,7 +34747,7 @@
         <v>2970</v>
       </c>
     </row>
-    <row r="2971" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2971" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2971" s="2" t="s">
         <v>2971</v>
       </c>
@@ -34752,31 +34755,31 @@
         <v>2971</v>
       </c>
     </row>
-    <row r="2972" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2972" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A2972" s="2" t="s">
         <v>2972</v>
       </c>
       <c r="B2972" s="1" t="s">
-        <v>2972</v>
-      </c>
-    </row>
-    <row r="2973" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3355</v>
+      </c>
+    </row>
+    <row r="2973" spans="1:3" ht="60" x14ac:dyDescent="0.25">
       <c r="A2973" s="2" t="s">
         <v>2973</v>
       </c>
       <c r="B2973" s="1" t="s">
-        <v>3358</v>
-      </c>
-    </row>
-    <row r="2974" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+        <v>3356</v>
+      </c>
+    </row>
+    <row r="2974" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2974" s="2" t="s">
         <v>2974</v>
       </c>
       <c r="B2974" s="1" t="s">
-        <v>3359</v>
-      </c>
-    </row>
-    <row r="2975" spans="1:2" x14ac:dyDescent="0.25">
+        <v>2974</v>
+      </c>
+    </row>
+    <row r="2975" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2975" s="2" t="s">
         <v>2975</v>
       </c>
@@ -34784,34 +34787,34 @@
         <v>2975</v>
       </c>
     </row>
-    <row r="2976" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="2976" spans="1:3" ht="75" x14ac:dyDescent="0.25">
       <c r="A2976" s="2" t="s">
         <v>2976</v>
       </c>
       <c r="B2976" s="1" t="s">
-        <v>2976</v>
-      </c>
-    </row>
-    <row r="2977" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+        <v>3357</v>
+      </c>
+      <c r="C2976" s="1" t="s">
+        <v>3358</v>
+      </c>
+    </row>
+    <row r="2977" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2977" s="2" t="s">
         <v>2977</v>
       </c>
       <c r="B2977" s="1" t="s">
+        <v>3359</v>
+      </c>
+      <c r="C2977" s="1" t="s">
         <v>3360</v>
       </c>
-      <c r="C2977" s="1" t="s">
-        <v>3361</v>
-      </c>
-    </row>
-    <row r="2978" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2978" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2978" s="2" t="s">
         <v>2978</v>
       </c>
       <c r="B2978" s="1" t="s">
-        <v>3362</v>
-      </c>
-      <c r="C2978" s="1" t="s">
-        <v>3363</v>
+        <v>2978</v>
       </c>
     </row>
     <row r="2979" spans="1:4" x14ac:dyDescent="0.25">
@@ -34822,26 +34825,26 @@
         <v>2979</v>
       </c>
     </row>
-    <row r="2980" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2980" spans="1:4" ht="60" x14ac:dyDescent="0.25">
       <c r="A2980" s="2" t="s">
         <v>2980</v>
       </c>
       <c r="B2980" s="1" t="s">
-        <v>2980</v>
-      </c>
-    </row>
-    <row r="2981" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+        <v>3361</v>
+      </c>
+      <c r="C2980" s="1" t="s">
+        <v>3362</v>
+      </c>
+      <c r="D2980" s="1" t="s">
+        <v>3363</v>
+      </c>
+    </row>
+    <row r="2981" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2981" s="2" t="s">
         <v>2981</v>
       </c>
       <c r="B2981" s="1" t="s">
-        <v>3364</v>
-      </c>
-      <c r="C2981" s="1" t="s">
-        <v>3365</v>
-      </c>
-      <c r="D2981" s="1" t="s">
-        <v>3366</v>
+        <v>2981</v>
       </c>
     </row>
     <row r="2982" spans="1:4" x14ac:dyDescent="0.25">
@@ -34924,37 +34927,38 @@
         <v>2991</v>
       </c>
     </row>
-    <row r="2992" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2992" spans="1:4" ht="30" x14ac:dyDescent="0.25">
       <c r="A2992" s="2" t="s">
         <v>2992</v>
       </c>
       <c r="B2992" s="1" t="s">
-        <v>2992</v>
-      </c>
-    </row>
-    <row r="2993" spans="1:3" x14ac:dyDescent="0.25">
+        <v>3328</v>
+      </c>
+    </row>
+    <row r="2993" spans="1:3" ht="90" x14ac:dyDescent="0.25">
       <c r="A2993" s="2" t="s">
         <v>2993</v>
       </c>
       <c r="B2993" s="1" t="s">
-        <v>2993</v>
-      </c>
-    </row>
-    <row r="2994" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>3329</v>
+      </c>
+    </row>
+    <row r="2994" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2994" s="2" t="s">
         <v>2994</v>
       </c>
       <c r="B2994" s="1" t="s">
-        <v>3331</v>
-      </c>
-    </row>
-    <row r="2995" spans="1:3" ht="90" x14ac:dyDescent="0.25">
+        <v>2994</v>
+      </c>
+    </row>
+    <row r="2995" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2995" s="2" t="s">
         <v>2995</v>
       </c>
       <c r="B2995" s="1" t="s">
-        <v>3332</v>
-      </c>
+        <v>2995</v>
+      </c>
+      <c r="C2995"/>
     </row>
     <row r="2996" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2996" s="2" t="s">
@@ -34963,6 +34967,7 @@
       <c r="B2996" s="1" t="s">
         <v>2996</v>
       </c>
+      <c r="C2996"/>
     </row>
     <row r="2997" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2997" s="2" t="s">
@@ -34971,15 +34976,18 @@
       <c r="B2997" s="1" t="s">
         <v>2997</v>
       </c>
-    </row>
-    <row r="2998" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C2997"/>
+    </row>
+    <row r="2998" spans="1:3" ht="120" x14ac:dyDescent="0.25">
       <c r="A2998" s="2" t="s">
         <v>2998</v>
       </c>
       <c r="B2998" s="1" t="s">
-        <v>2998</v>
-      </c>
-      <c r="C2998"/>
+        <v>3326</v>
+      </c>
+      <c r="C2998" s="1" t="s">
+        <v>3327</v>
+      </c>
     </row>
     <row r="2999" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2999" s="2" t="s">
@@ -34990,24 +34998,21 @@
       </c>
       <c r="C2999"/>
     </row>
-    <row r="3000" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3000" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A3000" s="2" t="s">
         <v>3000</v>
       </c>
       <c r="B3000" s="1" t="s">
-        <v>3000</v>
+        <v>3354</v>
       </c>
       <c r="C3000"/>
     </row>
-    <row r="3001" spans="1:3" ht="120" x14ac:dyDescent="0.25">
+    <row r="3001" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3001" s="2" t="s">
         <v>3001</v>
       </c>
       <c r="B3001" s="1" t="s">
-        <v>3329</v>
-      </c>
-      <c r="C3001" s="1" t="s">
-        <v>3330</v>
+        <v>3001</v>
       </c>
     </row>
     <row r="3002" spans="1:3" x14ac:dyDescent="0.25">
@@ -35017,16 +35022,14 @@
       <c r="B3002" s="1" t="s">
         <v>3002</v>
       </c>
-      <c r="C3002"/>
-    </row>
-    <row r="3003" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3003" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3003" s="2" t="s">
         <v>3003</v>
       </c>
       <c r="B3003" s="1" t="s">
-        <v>3357</v>
-      </c>
-      <c r="C3003"/>
+        <v>3003</v>
+      </c>
     </row>
     <row r="3004" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3004" s="2" t="s">
@@ -35132,7 +35135,7 @@
         <v>3016</v>
       </c>
     </row>
-    <row r="3017" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3017" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3017" s="2" t="s">
         <v>3017</v>
       </c>
@@ -35140,7 +35143,7 @@
         <v>3017</v>
       </c>
     </row>
-    <row r="3018" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3018" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3018" s="2" t="s">
         <v>3018</v>
       </c>
@@ -35148,7 +35151,7 @@
         <v>3018</v>
       </c>
     </row>
-    <row r="3019" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3019" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3019" s="2" t="s">
         <v>3019</v>
       </c>
@@ -35156,7 +35159,7 @@
         <v>3019</v>
       </c>
     </row>
-    <row r="3020" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3020" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3020" s="2" t="s">
         <v>3020</v>
       </c>
@@ -35188,7 +35191,7 @@
         <v>3023</v>
       </c>
     </row>
-    <row r="3024" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3024" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3024" s="2" t="s">
         <v>3024</v>
       </c>
@@ -35196,7 +35199,7 @@
         <v>3024</v>
       </c>
     </row>
-    <row r="3025" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3025" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3025" s="2" t="s">
         <v>3025</v>
       </c>
@@ -35212,7 +35215,7 @@
         <v>3026</v>
       </c>
     </row>
-    <row r="3027" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3027" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3027" s="2" t="s">
         <v>3027</v>
       </c>
@@ -35236,7 +35239,7 @@
         <v>3029</v>
       </c>
     </row>
-    <row r="3030" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3030" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3030" s="2" t="s">
         <v>3030</v>
       </c>
@@ -35492,7 +35495,7 @@
         <v>3061</v>
       </c>
     </row>
-    <row r="3062" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3062" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3062" s="2" t="s">
         <v>3062</v>
       </c>
@@ -35500,7 +35503,7 @@
         <v>3062</v>
       </c>
     </row>
-    <row r="3063" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3063" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3063" s="2" t="s">
         <v>3063</v>
       </c>
@@ -35516,7 +35519,7 @@
         <v>3064</v>
       </c>
     </row>
-    <row r="3065" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3065" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3065" s="2" t="s">
         <v>3065</v>
       </c>
@@ -35524,7 +35527,7 @@
         <v>3065</v>
       </c>
     </row>
-    <row r="3066" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3066" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3066" s="2" t="s">
         <v>3066</v>
       </c>
@@ -35653,7 +35656,7 @@
       </c>
     </row>
     <row r="3082" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3082" s="2" t="s">
+      <c r="A3082" s="1" t="s">
         <v>3082</v>
       </c>
       <c r="B3082" s="1" t="s">
@@ -35677,7 +35680,7 @@
       </c>
     </row>
     <row r="3085" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3085" s="1" t="s">
+      <c r="A3085" s="2" t="s">
         <v>3085</v>
       </c>
       <c r="B3085" s="1" t="s">
@@ -35844,7 +35847,7 @@
         <v>3105</v>
       </c>
     </row>
-    <row r="3106" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3106" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3106" s="2" t="s">
         <v>3106</v>
       </c>
@@ -35860,7 +35863,7 @@
         <v>3107</v>
       </c>
     </row>
-    <row r="3108" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3108" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3108" s="2" t="s">
         <v>3108</v>
       </c>
@@ -35876,7 +35879,7 @@
         <v>3109</v>
       </c>
     </row>
-    <row r="3110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3110" s="2" t="s">
         <v>3110</v>
       </c>
@@ -35884,7 +35887,7 @@
         <v>3110</v>
       </c>
     </row>
-    <row r="3111" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3111" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3111" s="2" t="s">
         <v>3111</v>
       </c>
@@ -35900,7 +35903,7 @@
         <v>3112</v>
       </c>
     </row>
-    <row r="3113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3113" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3113" s="2" t="s">
         <v>3113</v>
       </c>
@@ -35908,7 +35911,7 @@
         <v>3113</v>
       </c>
     </row>
-    <row r="3114" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3114" s="2" t="s">
         <v>3114</v>
       </c>
@@ -35932,7 +35935,7 @@
         <v>3116</v>
       </c>
     </row>
-    <row r="3117" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3117" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3117" s="2" t="s">
         <v>3117</v>
       </c>
@@ -35948,7 +35951,7 @@
         <v>3118</v>
       </c>
     </row>
-    <row r="3119" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3119" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3119" s="2" t="s">
         <v>3119</v>
       </c>
@@ -35956,7 +35959,7 @@
         <v>3119</v>
       </c>
     </row>
-    <row r="3120" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3120" s="2" t="s">
         <v>3120</v>
       </c>
@@ -36029,30 +36032,30 @@
       </c>
     </row>
     <row r="3129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3129" s="2" t="s">
+      <c r="A3129" s="1" t="s">
         <v>3129</v>
       </c>
       <c r="B3129" s="1" t="s">
         <v>3129</v>
       </c>
     </row>
-    <row r="3130" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3130" s="2" t="s">
+    <row r="3130" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3130" s="1" t="s">
         <v>3130</v>
       </c>
       <c r="B3130" s="1" t="s">
         <v>3130</v>
       </c>
     </row>
-    <row r="3131" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3131" s="2" t="s">
+    <row r="3131" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3131" s="1" t="s">
         <v>3131</v>
       </c>
       <c r="B3131" s="1" t="s">
         <v>3131</v>
       </c>
     </row>
-    <row r="3132" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3132" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3132" s="1" t="s">
         <v>3132</v>
       </c>
@@ -36076,7 +36079,7 @@
         <v>3134</v>
       </c>
     </row>
-    <row r="3135" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3135" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3135" s="1" t="s">
         <v>3135</v>
       </c>
@@ -36084,7 +36087,7 @@
         <v>3135</v>
       </c>
     </row>
-    <row r="3136" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3136" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3136" s="1" t="s">
         <v>3136</v>
       </c>
@@ -36100,7 +36103,7 @@
         <v>3137</v>
       </c>
     </row>
-    <row r="3138" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3138" s="1" t="s">
         <v>3138</v>
       </c>
@@ -36109,23 +36112,23 @@
       </c>
     </row>
     <row r="3139" spans="1:2" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3139" s="1" t="s">
+      <c r="A3139" s="2" t="s">
         <v>3139</v>
       </c>
       <c r="B3139" s="1" t="s">
         <v>3139</v>
       </c>
     </row>
-    <row r="3140" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3140" s="1" t="s">
+    <row r="3140" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3140" s="2" t="s">
         <v>3140</v>
       </c>
       <c r="B3140" s="1" t="s">
         <v>3140</v>
       </c>
     </row>
-    <row r="3141" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3141" s="1" t="s">
+    <row r="3141" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3141" s="2" t="s">
         <v>3141</v>
       </c>
       <c r="B3141" s="1" t="s">
@@ -36188,7 +36191,7 @@
         <v>3148</v>
       </c>
     </row>
-    <row r="3149" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3149" s="2" t="s">
         <v>3149</v>
       </c>
@@ -36204,7 +36207,7 @@
         <v>3150</v>
       </c>
     </row>
-    <row r="3151" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3151" s="2" t="s">
         <v>3151</v>
       </c>
@@ -36212,7 +36215,7 @@
         <v>3151</v>
       </c>
     </row>
-    <row r="3152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3152" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3152" s="2" t="s">
         <v>3152</v>
       </c>
@@ -36244,7 +36247,7 @@
         <v>3155</v>
       </c>
     </row>
-    <row r="3156" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3156" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3156" s="2" t="s">
         <v>3156</v>
       </c>
@@ -36252,7 +36255,7 @@
         <v>3156</v>
       </c>
     </row>
-    <row r="3157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3157" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3157" s="2" t="s">
         <v>3157</v>
       </c>
@@ -36260,7 +36263,7 @@
         <v>3157</v>
       </c>
     </row>
-    <row r="3158" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3158" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3158" s="2" t="s">
         <v>3158</v>
       </c>
@@ -36268,7 +36271,7 @@
         <v>3158</v>
       </c>
     </row>
-    <row r="3159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3159" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3159" s="2" t="s">
         <v>3159</v>
       </c>
@@ -36300,7 +36303,7 @@
         <v>3162</v>
       </c>
     </row>
-    <row r="3163" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3163" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3163" s="2" t="s">
         <v>3163</v>
       </c>
@@ -36324,7 +36327,7 @@
         <v>3165</v>
       </c>
     </row>
-    <row r="3166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3166" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A3166" s="2" t="s">
         <v>3166</v>
       </c>
@@ -36340,7 +36343,7 @@
         <v>3167</v>
       </c>
     </row>
-    <row r="3168" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="3168" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3168" s="2" t="s">
         <v>3168</v>
       </c>
@@ -36348,7 +36351,7 @@
         <v>3168</v>
       </c>
     </row>
-    <row r="3169" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3169" s="2" t="s">
         <v>3169</v>
       </c>
@@ -36356,7 +36359,7 @@
         <v>3169</v>
       </c>
     </row>
-    <row r="3170" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3170" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3170" s="2" t="s">
         <v>3170</v>
       </c>
@@ -36364,7 +36367,7 @@
         <v>3170</v>
       </c>
     </row>
-    <row r="3171" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3171" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3171" s="2" t="s">
         <v>3171</v>
       </c>
@@ -36372,7 +36375,7 @@
         <v>3171</v>
       </c>
     </row>
-    <row r="3172" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3172" s="2" t="s">
         <v>3172</v>
       </c>
@@ -36380,7 +36383,7 @@
         <v>3172</v>
       </c>
     </row>
-    <row r="3173" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3173" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3173" s="2" t="s">
         <v>3173</v>
       </c>
@@ -36388,7 +36391,7 @@
         <v>3173</v>
       </c>
     </row>
-    <row r="3174" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3174" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3174" s="2" t="s">
         <v>3174</v>
       </c>
@@ -36396,7 +36399,7 @@
         <v>3174</v>
       </c>
     </row>
-    <row r="3175" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3175" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3175" s="2" t="s">
         <v>3175</v>
       </c>
@@ -36404,7 +36407,7 @@
         <v>3175</v>
       </c>
     </row>
-    <row r="3176" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3176" s="2" t="s">
         <v>3176</v>
       </c>
@@ -36412,7 +36415,7 @@
         <v>3176</v>
       </c>
     </row>
-    <row r="3177" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3177" s="2" t="s">
         <v>3177</v>
       </c>
@@ -36420,7 +36423,7 @@
         <v>3177</v>
       </c>
     </row>
-    <row r="3178" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3178" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3178" s="2" t="s">
         <v>3178</v>
       </c>
@@ -36428,31 +36431,34 @@
         <v>3178</v>
       </c>
     </row>
-    <row r="3179" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="3179" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3179" s="2" t="s">
         <v>3179</v>
       </c>
       <c r="B3179" s="1" t="s">
         <v>3179</v>
       </c>
-    </row>
-    <row r="3180" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="C3179"/>
+    </row>
+    <row r="3180" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3180" s="2" t="s">
         <v>3180</v>
       </c>
       <c r="B3180" s="1" t="s">
         <v>3180</v>
       </c>
-    </row>
-    <row r="3181" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3180"/>
+    </row>
+    <row r="3181" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3181" s="2" t="s">
         <v>3181</v>
       </c>
       <c r="B3181" s="1" t="s">
         <v>3181</v>
       </c>
-    </row>
-    <row r="3182" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3181"/>
+    </row>
+    <row r="3182" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3182" s="2" t="s">
         <v>3182</v>
       </c>
@@ -36461,7 +36467,7 @@
       </c>
       <c r="C3182"/>
     </row>
-    <row r="3183" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="3183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3183" s="2" t="s">
         <v>3183</v>
       </c>
@@ -36470,199 +36476,172 @@
       </c>
       <c r="C3183"/>
     </row>
-    <row r="3184" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3184" s="2" t="s">
-        <v>3184</v>
+    <row r="3184" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+      <c r="A3184" s="1" t="s">
+        <v>1578</v>
       </c>
       <c r="B3184" s="1" t="s">
         <v>3184</v>
       </c>
-      <c r="C3184"/>
-    </row>
-    <row r="3185" spans="1:7" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3185" s="2" t="s">
+      <c r="D3184" s="1"/>
+      <c r="E3184" s="1"/>
+      <c r="F3184" s="1"/>
+      <c r="G3184" s="1"/>
+    </row>
+    <row r="3185" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+      <c r="A3185" s="1" t="s">
+        <v>2858</v>
+      </c>
+      <c r="B3185" s="1" t="s">
+        <v>3186</v>
+      </c>
+      <c r="C3185" s="1" t="s">
         <v>3185</v>
       </c>
-      <c r="B3185" s="1" t="s">
-        <v>3185</v>
-      </c>
-      <c r="C3185"/>
-    </row>
-    <row r="3186" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A3186" s="2" t="s">
-        <v>3186</v>
+      <c r="D3185" s="1"/>
+      <c r="E3185" s="1"/>
+      <c r="F3185" s="1"/>
+      <c r="G3185" s="1"/>
+    </row>
+    <row r="3186" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3186" s="1" t="s">
+        <v>30</v>
       </c>
       <c r="B3186" s="1" t="s">
-        <v>3186</v>
-      </c>
-      <c r="C3186"/>
-    </row>
-    <row r="3187" spans="1:7" ht="90" x14ac:dyDescent="0.25">
+        <v>3187</v>
+      </c>
+      <c r="D3186" s="1"/>
+      <c r="E3186" s="1"/>
+      <c r="F3186" s="1"/>
+      <c r="G3186" s="1"/>
+    </row>
+    <row r="3187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3187" s="1" t="s">
-        <v>1578</v>
+        <v>3246</v>
       </c>
       <c r="B3187" s="1" t="s">
-        <v>3187</v>
-      </c>
-      <c r="D3187" s="1"/>
-      <c r="E3187" s="1"/>
-      <c r="F3187" s="1"/>
-      <c r="G3187" s="1"/>
-    </row>
-    <row r="3188" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>3247</v>
+      </c>
+    </row>
+    <row r="3188" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3188" s="1" t="s">
-        <v>2859</v>
+        <v>3258</v>
       </c>
       <c r="B3188" s="1" t="s">
-        <v>3189</v>
-      </c>
-      <c r="C3188" s="1" t="s">
-        <v>3188</v>
-      </c>
-      <c r="D3188" s="1"/>
-      <c r="E3188" s="1"/>
-      <c r="F3188" s="1"/>
-      <c r="G3188" s="1"/>
+        <v>3259</v>
+      </c>
     </row>
     <row r="3189" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3189" s="1" t="s">
-        <v>30</v>
+        <v>3280</v>
       </c>
       <c r="B3189" s="1" t="s">
-        <v>3190</v>
-      </c>
-      <c r="D3189" s="1"/>
-      <c r="E3189" s="1"/>
-      <c r="F3189" s="1"/>
-      <c r="G3189" s="1"/>
-    </row>
-    <row r="3190" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3281</v>
+      </c>
+    </row>
+    <row r="3190" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3190" s="1" t="s">
-        <v>3249</v>
+        <v>3282</v>
       </c>
       <c r="B3190" s="1" t="s">
-        <v>3250</v>
+        <v>3283</v>
       </c>
     </row>
     <row r="3191" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3191" s="1" t="s">
-        <v>3261</v>
+        <v>3284</v>
       </c>
       <c r="B3191" s="1" t="s">
-        <v>3262</v>
-      </c>
-    </row>
-    <row r="3192" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>3285</v>
+      </c>
+    </row>
+    <row r="3192" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3192" s="1" t="s">
-        <v>3283</v>
+        <v>3286</v>
       </c>
       <c r="B3192" s="1" t="s">
-        <v>3284</v>
+        <v>3287</v>
       </c>
     </row>
     <row r="3193" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3193" s="1" t="s">
-        <v>3285</v>
+        <v>3288</v>
       </c>
       <c r="B3193" s="1" t="s">
-        <v>3286</v>
-      </c>
-    </row>
-    <row r="3194" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>3289</v>
+      </c>
+    </row>
+    <row r="3194" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3194" s="1" t="s">
-        <v>3287</v>
+        <v>3290</v>
       </c>
       <c r="B3194" s="1" t="s">
-        <v>3288</v>
-      </c>
-    </row>
-    <row r="3195" spans="1:7" x14ac:dyDescent="0.25">
+        <v>3291</v>
+      </c>
+    </row>
+    <row r="3195" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3195" s="1" t="s">
-        <v>3289</v>
+        <v>3293</v>
       </c>
       <c r="B3195" s="1" t="s">
-        <v>3290</v>
+        <v>3294</v>
       </c>
     </row>
     <row r="3196" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3196" s="1" t="s">
-        <v>3291</v>
+        <v>3292</v>
       </c>
       <c r="B3196" s="1" t="s">
-        <v>3292</v>
-      </c>
-    </row>
-    <row r="3197" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+        <v>3294</v>
+      </c>
+    </row>
+    <row r="3197" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A3197" s="1" t="s">
-        <v>3293</v>
+        <v>3295</v>
       </c>
       <c r="B3197" s="1" t="s">
-        <v>3294</v>
+        <v>3296</v>
       </c>
     </row>
     <row r="3198" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3198" s="1" t="s">
-        <v>3296</v>
+        <v>3297</v>
       </c>
       <c r="B3198" s="1" t="s">
-        <v>3297</v>
+        <v>3299</v>
       </c>
     </row>
     <row r="3199" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A3199" s="1" t="s">
-        <v>3295</v>
+        <v>3298</v>
       </c>
       <c r="B3199" s="1" t="s">
-        <v>3297</v>
-      </c>
-    </row>
-    <row r="3200" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+        <v>3299</v>
+      </c>
+    </row>
+    <row r="3200" spans="1:7" ht="60" x14ac:dyDescent="0.25">
       <c r="A3200" s="1" t="s">
-        <v>3298</v>
+        <v>3300</v>
       </c>
       <c r="B3200" s="1" t="s">
-        <v>3299</v>
-      </c>
-    </row>
-    <row r="3201" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3302</v>
+      </c>
+    </row>
+    <row r="3201" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A3201" s="1" t="s">
-        <v>3300</v>
+        <v>3301</v>
       </c>
       <c r="B3201" s="1" t="s">
-        <v>3302</v>
-      </c>
-    </row>
-    <row r="3202" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>3303</v>
+      </c>
+    </row>
+    <row r="3202" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3202" s="1" t="s">
-        <v>3301</v>
-      </c>
-      <c r="B3202" s="1" t="s">
-        <v>3302</v>
-      </c>
-    </row>
-    <row r="3203" spans="1:2" ht="60" x14ac:dyDescent="0.25">
-      <c r="A3203" s="1" t="s">
-        <v>3303</v>
-      </c>
-      <c r="B3203" s="1" t="s">
-        <v>3305</v>
-      </c>
-    </row>
-    <row r="3204" spans="1:2" ht="75" x14ac:dyDescent="0.25">
-      <c r="A3204" s="1" t="s">
-        <v>3304</v>
-      </c>
-      <c r="B3204" s="1" t="s">
-        <v>3306</v>
-      </c>
-    </row>
-    <row r="3205" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3205" s="1" t="s">
-        <v>3316</v>
+        <v>3313</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A2:G3189" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
+  <autoFilter ref="A2:G3202" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
   <conditionalFormatting sqref="A1:A1048576">
     <cfRule type="duplicateValues" dxfId="38" priority="7"/>
@@ -36682,26 +36661,26 @@
   <conditionalFormatting sqref="A145:A208">
     <cfRule type="duplicateValues" dxfId="31" priority="111"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1623:A1625 A1:C172 A174:C176 A173 C173 A178:C180 A177 C177 A182:C184 A181 C181 A186:C188 A185 C185 A189 C189 C1623:C1625 A190:C204 A1626:C1691 A1692:A1706 C1692:C1706 A1707:C1755 A1757:C1757 A1756 C1756 A1763:C1763 A1762 C1762 A1759:C1761 A1758 C1758 A1764 C1764 A205 C205 A1765:C1048576 A206:C1622">
+  <conditionalFormatting sqref="A1622:A1624 A1:C172 A174:C176 A173 C173 A178:C180 A177 C177 A182:C184 A181 C181 A186:C188 A185 C185 A189 C189 C1622:C1624 A190:C204 A1625:C1690 A1691:A1705 C1691:C1705 A1706:C1754 A1756:C1756 A1755 C1755 A1762:C1762 A1761 C1761 A1758:C1760 A1757 C1757 A1763 C1763 A205 C205 A1764:C1048576 A206:C1621">
     <cfRule type="duplicateValues" dxfId="30" priority="6"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2571:A2809 A1554">
+  <conditionalFormatting sqref="A2570:A2808 A1554">
     <cfRule type="duplicateValues" dxfId="29" priority="73"/>
     <cfRule type="duplicateValues" dxfId="28" priority="74"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A2970:A2974">
+  <conditionalFormatting sqref="A2969:A2973">
     <cfRule type="duplicateValues" dxfId="27" priority="5481"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3190:A1048576 A2:A3186">
+  <conditionalFormatting sqref="A3187:A1048576 A2:A3183">
     <cfRule type="duplicateValues" dxfId="26" priority="13"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3190:A1048576 A2:A3187">
+  <conditionalFormatting sqref="A3187:A1048576 A2:A3184">
     <cfRule type="duplicateValues" dxfId="25" priority="11"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A3190:A1048576 A2:A3188">
+  <conditionalFormatting sqref="A3187:A1048576 A2:A3185">
     <cfRule type="duplicateValues" dxfId="24" priority="9"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A5514:A1048576 A2810:A2969 A209:A1540 A2:A23 A25:A84 A143 A2975:A2999">
+  <conditionalFormatting sqref="A5511:A1048576 A2809:A2968 A209:A1540 A2:A23 A25:A84 A143 A2974:A2996">
     <cfRule type="duplicateValues" dxfId="23" priority="151"/>
     <cfRule type="duplicateValues" dxfId="22" priority="153"/>
   </conditionalFormatting>
@@ -36735,31 +36714,31 @@
   <conditionalFormatting sqref="B1541">
     <cfRule type="duplicateValues" dxfId="10" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B1626:B1691 B1707:B1755 B1757 B1763 B1759:B1761 B1765:B2468 B1555:B1622">
+  <conditionalFormatting sqref="B1625:B1690 B1706:B1754 B1756 B1762 B1758:B1760 B1764:B2467 B1555:B1621">
     <cfRule type="duplicateValues" dxfId="9" priority="369"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2571:B2809 B1554">
+  <conditionalFormatting sqref="B2570:B2808 B1554">
     <cfRule type="duplicateValues" dxfId="8" priority="16"/>
     <cfRule type="duplicateValues" dxfId="7" priority="17"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2970:B2974">
+  <conditionalFormatting sqref="B2969:B2973">
     <cfRule type="duplicateValues" dxfId="6" priority="5482"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B5514:B1048576 B2:B23 B25:B84 B143 B2975:B2999 B2810:B2969 B209:B1540">
+  <conditionalFormatting sqref="B5511:B1048576 B2:B23 B25:B84 B143 B2974:B2996 B2809:B2968 B209:B1540">
     <cfRule type="duplicateValues" dxfId="5" priority="25"/>
     <cfRule type="duplicateValues" dxfId="4" priority="26"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3187:W3187">
+  <conditionalFormatting sqref="G3184:W3184">
     <cfRule type="duplicateValues" dxfId="3" priority="12"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3188:W3188">
+  <conditionalFormatting sqref="G3185:W3185">
     <cfRule type="duplicateValues" dxfId="2" priority="10"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="G3189:W3189">
+  <conditionalFormatting sqref="G3186:W3186">
     <cfRule type="duplicateValues" dxfId="1" priority="8"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1555:A2468">
-    <cfRule type="duplicateValues" dxfId="0" priority="5572"/>
+  <conditionalFormatting sqref="A1555:A2467">
+    <cfRule type="duplicateValues" dxfId="0" priority="5576"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>